<commit_message>
Update replace_user form to support using it at all levels of the default hierarchy
</commit_message>
<xml_diff>
--- a/config/default/forms/app/replace_user.xlsx
+++ b/config/default/forms/app/replace_user.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
   <si>
     <t>type</t>
   </si>
@@ -176,10 +176,13 @@
     <t>parent</t>
   </si>
   <si>
-    <t xml:space="preserve">Household ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area ID</t>
+    <t xml:space="preserve">Parent 1 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent 2 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent 3 ID</t>
   </si>
   <si>
     <t>calculate</t>
@@ -194,16 +197,22 @@
     <t>../inputs/contact/_id</t>
   </si>
   <si>
-    <t>contact_area_id</t>
+    <t>parent_1_id</t>
   </si>
   <si>
     <t>../inputs/contact/parent/_id</t>
   </si>
   <si>
-    <t>contact_facility_id</t>
+    <t>parent_2_id</t>
   </si>
   <si>
     <t>../inputs/contact/parent/parent/_id</t>
+  </si>
+  <si>
+    <t>parent_3_id</t>
+  </si>
+  <si>
+    <t>../inputs/contact/parent/parent/parent/_id</t>
   </si>
   <si>
     <t>user_phone</t>
@@ -279,16 +288,19 @@
     <t xml:space="preserve">New User</t>
   </si>
   <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>${contact_area_id}</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>${contact_facility_id}</t>
+    <t>${parent_1_id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${parent_2_id} != ''</t>
+  </si>
+  <si>
+    <t>${parent_2_id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${parent_3_id} != ''</t>
+  </si>
+  <si>
+    <t>${parent_3_id}</t>
   </si>
   <si>
     <t>Type</t>
@@ -453,7 +465,7 @@
     <t>phone_read_only</t>
   </si>
   <si>
-    <t>boolean(${user_phone})</t>
+    <t xml:space="preserve">${user_phone} != ''</t>
   </si>
   <si>
     <t>${user_phone}</t>
@@ -468,7 +480,7 @@
     <t>new_phone</t>
   </si>
   <si>
-    <t>not(boolean(${user_phone}))</t>
+    <t xml:space="preserve">${user_phone} = ''</t>
   </si>
   <si>
     <t xml:space="preserve">Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +254712345678</t>
@@ -1264,7 +1276,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{5C008D89-1249-1821-A035-20B9C9B30380}"/>
+  <person displayName=" " id="{F68F2BEC-0C94-05D9-E827-15E919827533}"/>
 </personList>
 </file>
 
@@ -1680,7 +1692,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="M1" personId="{5C008D89-1249-1821-A035-20B9C9B30380}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
+  <threadedComment ref="M1" personId="{F68F2BEC-0C94-05D9-E827-15E919827533}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
     <text xml:space="preserve">Comment:
 +marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
@@ -2151,9 +2163,7 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -2195,12 +2205,14 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -2219,12 +2231,14 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -2246,7 +2260,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -2270,7 +2284,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -2284,118 +2298,118 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="A22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="14"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+      <c r="A23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="A24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J25" s="14"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="14"/>
+        <v>45</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="15" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="16"/>
@@ -2407,10 +2421,10 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -2419,7 +2433,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="16"/>
@@ -2428,42 +2442,26 @@
       <c r="N27" s="15"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
-      <c r="AF27" s="1"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
       <c r="I28" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="1"/>
@@ -2471,23 +2469,23 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="14"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="1"/>
@@ -2495,233 +2493,251 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="14"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" ht="15">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="14"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-    </row>
-    <row r="32" ht="15">
-      <c r="A32" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G32" s="19"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="N32" s="19"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
+    <row r="35" ht="15">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
     <row r="36" ht="15">
       <c r="A36" s="17" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="18"/>
+        <v>64</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+      <c r="F36" s="19" t="s">
+        <v>65</v>
+      </c>
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
       <c r="J36" s="18"/>
       <c r="K36" s="19"/>
       <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
+      <c r="M36" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="N36" s="19"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" ht="15">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
+    <row r="37" ht="12.75" customHeight="1">
+      <c r="A37" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="19"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
-      <c r="F38" s="19" t="s">
-        <v>18</v>
-      </c>
+      <c r="F38" s="19"/>
       <c r="G38" s="19"/>
       <c r="H38" s="18"/>
       <c r="I38" s="19"/>
       <c r="J38" s="18"/>
       <c r="K38" s="19"/>
       <c r="L38" s="19"/>
-      <c r="M38" s="19" t="s">
-        <v>63</v>
-      </c>
+      <c r="M38" s="19"/>
       <c r="N38" s="19"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="19" t="s">
-        <v>19</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="18"/>
       <c r="I39" s="19"/>
@@ -2733,24 +2749,20 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" ht="15">
       <c r="A40" s="17" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>75</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C40" s="18"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
       <c r="H40" s="18"/>
-      <c r="I40" s="19" t="s">
-        <v>76</v>
-      </c>
+      <c r="I40" s="19"/>
       <c r="J40" s="18"/>
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
@@ -2759,69 +2771,67 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="19"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
+    <row r="41" ht="15">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
+      <c r="F42" s="19" t="s">
+        <v>18</v>
+      </c>
       <c r="G42" s="19"/>
       <c r="H42" s="18"/>
-      <c r="I42" s="19" t="s">
-        <v>78</v>
-      </c>
+      <c r="I42" s="19"/>
       <c r="J42" s="18"/>
       <c r="K42" s="19"/>
       <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
+      <c r="M42" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="N42" s="19"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="18"/>
+      <c r="C43" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="D43" s="19"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="19"/>
+      <c r="F43" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="G43" s="19"/>
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
@@ -2835,18 +2845,22 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="17" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="18"/>
+        <v>35</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="D44" s="19"/>
-      <c r="E44" s="18"/>
+      <c r="E44" s="19"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
       <c r="H44" s="18"/>
-      <c r="I44" s="19"/>
+      <c r="I44" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="J44" s="18"/>
       <c r="K44" s="19"/>
       <c r="L44" s="19"/>
@@ -2857,22 +2871,24 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C45" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="E45" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
+      <c r="F45" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="G45" s="19"/>
       <c r="H45" s="18"/>
-      <c r="I45" s="20" t="s">
-        <v>80</v>
-      </c>
+      <c r="I45" s="19"/>
       <c r="J45" s="18"/>
       <c r="K45" s="19"/>
       <c r="L45" s="19"/>
@@ -2883,22 +2899,22 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="17" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>72</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
       <c r="H46" s="18"/>
-      <c r="I46" s="19"/>
+      <c r="I46" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="J46" s="18"/>
       <c r="K46" s="19"/>
       <c r="L46" s="19"/>
@@ -2909,27 +2925,23 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="17" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
+      <c r="E47" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="F47" s="19"/>
-      <c r="G47" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>85</v>
-      </c>
+      <c r="G47" s="19"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="19"/>
-      <c r="J47" s="18" t="s">
-        <v>86</v>
-      </c>
+      <c r="J47" s="18"/>
       <c r="K47" s="19"/>
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
@@ -2939,21 +2951,21 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="19" t="s">
-        <v>72</v>
-      </c>
+      <c r="D48" s="19"/>
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
       <c r="H48" s="18"/>
       <c r="I48" s="19" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J48" s="18"/>
       <c r="K48" s="19"/>
@@ -2965,10 +2977,10 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="17" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="19"/>
@@ -2976,9 +2988,7 @@
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
       <c r="H49" s="18"/>
-      <c r="I49" s="19" t="s">
-        <v>90</v>
-      </c>
+      <c r="I49" s="19"/>
       <c r="J49" s="18"/>
       <c r="K49" s="19"/>
       <c r="L49" s="19"/>
@@ -2989,16 +2999,14 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="17" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>16</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C50" s="18"/>
       <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
+      <c r="E50" s="18"/>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
       <c r="H50" s="18"/>
@@ -3013,31 +3021,19 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="17" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>95</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="18"/>
       <c r="F51" s="19"/>
-      <c r="G51" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>97</v>
-      </c>
+      <c r="G51" s="19"/>
+      <c r="H51" s="18"/>
       <c r="I51" s="19"/>
-      <c r="J51" s="18" t="s">
-        <v>98</v>
-      </c>
+      <c r="J51" s="18"/>
       <c r="K51" s="19"/>
       <c r="L51" s="19"/>
       <c r="M51" s="19"/>
@@ -3047,22 +3043,22 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="17" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D52" s="19"/>
-      <c r="E52" s="19" t="s">
-        <v>101</v>
-      </c>
+      <c r="E52" s="19"/>
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
       <c r="H52" s="18"/>
-      <c r="I52" s="19"/>
+      <c r="I52" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="J52" s="18"/>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
@@ -3073,27 +3069,21 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>101</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E53" s="19"/>
       <c r="F53" s="19"/>
-      <c r="G53" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="H53" s="18" t="s">
-        <v>106</v>
-      </c>
+      <c r="G53" s="19"/>
+      <c r="H53" s="18"/>
       <c r="I53" s="19"/>
       <c r="J53" s="18"/>
       <c r="K53" s="19"/>
@@ -3105,27 +3095,27 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="17" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D54" s="19"/>
-      <c r="E54" s="19" t="s">
-        <v>101</v>
-      </c>
+      <c r="E54" s="19"/>
       <c r="F54" s="19"/>
       <c r="G54" s="19" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="I54" s="19"/>
-      <c r="J54" s="18"/>
+      <c r="J54" s="18" t="s">
+        <v>90</v>
+      </c>
       <c r="K54" s="19"/>
       <c r="L54" s="19"/>
       <c r="M54" s="19"/>
@@ -3135,22 +3125,22 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="17" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="19"/>
+        <v>91</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="E55" s="19"/>
-      <c r="F55" s="19" t="s">
-        <v>113</v>
-      </c>
+      <c r="F55" s="19"/>
       <c r="G55" s="19"/>
       <c r="H55" s="18"/>
-      <c r="I55" s="19"/>
+      <c r="I55" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="J55" s="18"/>
       <c r="K55" s="19"/>
       <c r="L55" s="19"/>
@@ -3161,10 +3151,10 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="19"/>
@@ -3173,7 +3163,7 @@
       <c r="G56" s="19"/>
       <c r="H56" s="18"/>
       <c r="I56" s="19" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="J56" s="18"/>
       <c r="K56" s="19"/>
@@ -3185,20 +3175,20 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C57" s="18"/>
+        <v>95</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="D57" s="19"/>
       <c r="E57" s="19"/>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
       <c r="H57" s="18"/>
-      <c r="I57" s="19" t="s">
-        <v>117</v>
-      </c>
+      <c r="I57" s="19"/>
       <c r="J57" s="18"/>
       <c r="K57" s="19"/>
       <c r="L57" s="19"/>
@@ -3209,21 +3199,31 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="17" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="J58" s="18"/>
+      <c r="G58" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I58" s="19"/>
+      <c r="J58" s="18" t="s">
+        <v>102</v>
+      </c>
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
       <c r="M58" s="19"/>
@@ -3233,20 +3233,22 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="17" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="18"/>
+        <v>103</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
+      <c r="E59" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
       <c r="H59" s="18"/>
-      <c r="I59" s="18" t="s">
-        <v>121</v>
-      </c>
+      <c r="I59" s="19"/>
       <c r="J59" s="18"/>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
@@ -3257,20 +3259,28 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="17" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
+        <v>107</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="19" t="s">
-        <v>123</v>
-      </c>
+      <c r="G60" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="I60" s="19"/>
       <c r="J60" s="18"/>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
@@ -3281,21 +3291,25 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="17" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="19" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="18"/>
+      <c r="G61" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="I61" s="19"/>
       <c r="J61" s="18"/>
       <c r="K61" s="19"/>
@@ -3307,15 +3321,19 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="18"/>
+        <v>116</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
+      <c r="F62" s="19" t="s">
+        <v>117</v>
+      </c>
       <c r="G62" s="19"/>
       <c r="H62" s="18"/>
       <c r="I62" s="19"/>
@@ -3329,24 +3347,20 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>72</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C63" s="18"/>
+      <c r="D63" s="19"/>
       <c r="E63" s="19"/>
-      <c r="F63" s="19" t="s">
-        <v>113</v>
-      </c>
+      <c r="F63" s="19"/>
       <c r="G63" s="19"/>
       <c r="H63" s="18"/>
-      <c r="I63" s="19"/>
+      <c r="I63" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="J63" s="18"/>
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
@@ -3357,31 +3371,23 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="17" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>31</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C64" s="18"/>
       <c r="D64" s="19"/>
-      <c r="E64" s="19" t="s">
-        <v>131</v>
-      </c>
+      <c r="E64" s="19"/>
       <c r="F64" s="19"/>
       <c r="G64" s="19"/>
       <c r="H64" s="18"/>
       <c r="I64" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="J64" s="18" t="s">
-        <v>133</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="J64" s="18"/>
       <c r="K64" s="19"/>
-      <c r="L64" s="19" t="s">
-        <v>72</v>
-      </c>
+      <c r="L64" s="19"/>
       <c r="M64" s="19"/>
       <c r="N64" s="19"/>
       <c r="O64" s="1"/>
@@ -3389,28 +3395,20 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D65" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>136</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C65" s="18"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
       <c r="F65" s="19"/>
-      <c r="G65" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H65" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="I65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="19" t="s">
+        <v>123</v>
+      </c>
       <c r="J65" s="18"/>
       <c r="K65" s="19"/>
       <c r="L65" s="19"/>
@@ -3421,21 +3419,19 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>31</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C66" s="18"/>
       <c r="D66" s="19"/>
       <c r="E66" s="19"/>
       <c r="F66" s="19"/>
       <c r="G66" s="19"/>
       <c r="H66" s="18"/>
-      <c r="I66" s="19" t="s">
-        <v>138</v>
+      <c r="I66" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="J66" s="18"/>
       <c r="K66" s="19"/>
@@ -3447,24 +3443,20 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="17" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>140</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C67" s="18"/>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
       <c r="F67" s="19"/>
-      <c r="G67" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H67" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="I67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="19" t="s">
+        <v>127</v>
+      </c>
       <c r="J67" s="18"/>
       <c r="K67" s="19"/>
       <c r="L67" s="19"/>
@@ -3472,81 +3464,41 @@
       <c r="N67" s="19"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1"/>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="1"/>
-      <c r="AD67" s="1"/>
-      <c r="AE67" s="1"/>
-      <c r="AF67" s="1"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="17" t="s">
-        <v>141</v>
+        <v>67</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19" t="s">
-        <v>142</v>
-      </c>
+      <c r="E68" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="19"/>
       <c r="G68" s="19"/>
       <c r="H68" s="18"/>
-      <c r="I68" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="J68" s="18" t="s">
-        <v>133</v>
-      </c>
+      <c r="I68" s="19"/>
+      <c r="J68" s="18"/>
       <c r="K68" s="19"/>
-      <c r="L68" s="19" t="s">
-        <v>72</v>
-      </c>
+      <c r="L68" s="19"/>
       <c r="M68" s="19"/>
       <c r="N68" s="19"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-      <c r="Z68" s="1"/>
-      <c r="AA68" s="1"/>
-      <c r="AB68" s="1"/>
-      <c r="AC68" s="1"/>
-      <c r="AD68" s="1"/>
-      <c r="AE68" s="1"/>
-      <c r="AF68" s="1"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>145</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C69" s="18"/>
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
       <c r="F69" s="19"/>
@@ -3560,37 +3512,23 @@
       <c r="N69" s="19"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="1"/>
-      <c r="V69" s="1"/>
-      <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-      <c r="AA69" s="1"/>
-      <c r="AB69" s="1"/>
-      <c r="AC69" s="1"/>
-      <c r="AD69" s="1"/>
-      <c r="AE69" s="1"/>
-      <c r="AF69" s="1"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="17" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="19"/>
+        <v>132</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="E70" s="19"/>
       <c r="F70" s="19" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="G70" s="19"/>
       <c r="H70" s="18"/>
@@ -3605,23 +3543,31 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="17" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C71" s="18"/>
+        <v>134</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
+      <c r="E71" s="19" t="s">
+        <v>135</v>
+      </c>
       <c r="F71" s="19"/>
       <c r="G71" s="19"/>
       <c r="H71" s="18"/>
       <c r="I71" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="J71" s="18"/>
+        <v>136</v>
+      </c>
+      <c r="J71" s="18" t="s">
+        <v>137</v>
+      </c>
       <c r="K71" s="19"/>
-      <c r="L71" s="19"/>
+      <c r="L71" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="M71" s="19"/>
       <c r="N71" s="19"/>
       <c r="O71" s="1"/>
@@ -3629,20 +3575,28 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="17" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C72" s="18"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
+        <v>139</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>140</v>
+      </c>
       <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="19" t="s">
-        <v>148</v>
-      </c>
+      <c r="G72" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I72" s="19"/>
       <c r="J72" s="18"/>
       <c r="K72" s="19"/>
       <c r="L72" s="19"/>
@@ -3653,19 +3607,21 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C73" s="18"/>
+        <v>30</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
       <c r="F73" s="19"/>
       <c r="G73" s="19"/>
       <c r="H73" s="18"/>
       <c r="I73" s="19" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="J73" s="18"/>
       <c r="K73" s="19"/>
@@ -3677,17 +3633,23 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="17" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C74" s="18"/>
+        <v>143</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>144</v>
+      </c>
       <c r="D74" s="19"/>
       <c r="E74" s="19"/>
       <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="18"/>
+      <c r="G74" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H74" s="18" t="s">
+        <v>141</v>
+      </c>
       <c r="I74" s="19"/>
       <c r="J74" s="18"/>
       <c r="K74" s="19"/>
@@ -3696,47 +3658,87 @@
       <c r="N74" s="19"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
+      <c r="AC74" s="1"/>
+      <c r="AD74" s="1"/>
+      <c r="AE74" s="1"/>
+      <c r="AF74" s="1"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="17" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C75" s="18"/>
+        <v>38</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="D75" s="19"/>
       <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
+      <c r="F75" s="19" t="s">
+        <v>146</v>
+      </c>
       <c r="G75" s="19"/>
       <c r="H75" s="18"/>
       <c r="I75" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="J75" s="18"/>
+        <v>147</v>
+      </c>
+      <c r="J75" s="18" t="s">
+        <v>137</v>
+      </c>
       <c r="K75" s="19"/>
-      <c r="L75" s="19"/>
+      <c r="L75" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="M75" s="19"/>
-      <c r="N75" s="19" t="s">
-        <v>152</v>
-      </c>
+      <c r="N75" s="19"/>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+      <c r="AC75" s="1"/>
+      <c r="AD75" s="1"/>
+      <c r="AE75" s="1"/>
+      <c r="AF75" s="1"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="18"/>
+        <v>148</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>149</v>
+      </c>
       <c r="D76" s="19"/>
       <c r="E76" s="19"/>
       <c r="F76" s="19"/>
       <c r="G76" s="19"/>
       <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
+      <c r="I76" s="19"/>
       <c r="J76" s="18"/>
       <c r="K76" s="19"/>
       <c r="L76" s="19"/>
@@ -3744,31 +3746,55 @@
       <c r="N76" s="19"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="1"/>
+      <c r="AB76" s="1"/>
+      <c r="AC76" s="1"/>
+      <c r="AD76" s="1"/>
+      <c r="AE76" s="1"/>
+      <c r="AF76" s="1"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="10"/>
-      <c r="I77" s="10"/>
-      <c r="J77" s="10"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
+      <c r="A77" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G77" s="19"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="19"/>
+      <c r="L77" s="19"/>
+      <c r="M77" s="19"/>
+      <c r="N77" s="19"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="19"/>
@@ -3776,23 +3802,23 @@
       <c r="F78" s="19"/>
       <c r="G78" s="19"/>
       <c r="H78" s="18"/>
-      <c r="I78" s="18" t="s">
-        <v>46</v>
+      <c r="I78" s="19" t="s">
+        <v>151</v>
       </c>
       <c r="J78" s="18"/>
       <c r="K78" s="19"/>
       <c r="L78" s="19"/>
       <c r="M78" s="19"/>
-      <c r="N78" s="18"/>
+      <c r="N78" s="19"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>154</v>
+        <v>60</v>
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="19"/>
@@ -3800,18 +3826,178 @@
       <c r="F79" s="19"/>
       <c r="G79" s="19"/>
       <c r="H79" s="18"/>
-      <c r="I79" s="18" t="s">
-        <v>155</v>
+      <c r="I79" s="19" t="s">
+        <v>152</v>
       </c>
       <c r="J79" s="18"/>
       <c r="K79" s="19"/>
       <c r="L79" s="19"/>
       <c r="M79" s="19"/>
-      <c r="N79" s="18" t="s">
-        <v>155</v>
-      </c>
+      <c r="N79" s="19"/>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" s="18"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="J80" s="18"/>
+      <c r="K80" s="19"/>
+      <c r="L80" s="19"/>
+      <c r="M80" s="19"/>
+      <c r="N80" s="19"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+    </row>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="A81" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="18"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="19"/>
+      <c r="L81" s="19"/>
+      <c r="M81" s="19"/>
+      <c r="N81" s="19"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="18"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="J82" s="18"/>
+      <c r="K82" s="19"/>
+      <c r="L82" s="19"/>
+      <c r="M82" s="19"/>
+      <c r="N82" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C83" s="18"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="19"/>
+      <c r="L83" s="19"/>
+      <c r="M83" s="19"/>
+      <c r="N83" s="19"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+    </row>
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="A84" s="10"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+    </row>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B85" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C85" s="18"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J85" s="18"/>
+      <c r="K85" s="19"/>
+      <c r="L85" s="19"/>
+      <c r="M85" s="19"/>
+      <c r="N85" s="18"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+    </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86" s="18"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="J86" s="18"/>
+      <c r="K86" s="19"/>
+      <c r="L86" s="19"/>
+      <c r="M86" s="19"/>
+      <c r="N86" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -3822,79 +4008,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="21" disablePrompts="0">
-        <x14:dataValidation xr:uid="{002E004D-00AB-4B20-891F-004A004500D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0089006D-0001-4BE3-9625-004A00F4008B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D2:D8 D10 D21:D22 D24 D31 D37:D46 D74:D75 D76:D77</xm:sqref>
+          <xm:sqref>D2:D8 D10 D24:D25 D35 D41:D53 D81:D82 D83:D84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A30028-00D9-448B-954E-00E1004600EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{007000BF-001F-431C-9A34-001200B2001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A1:A2 A6:A8 A10 A21:A22 A24 A31 A37:A46 A74:A75 A76:A77</xm:sqref>
+          <xm:sqref>A1:A2 A6:A8 A10 A24:A25 A35 A41:A53 A81:A82 A83:A84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DA00AF-00BC-4A65-99A1-008E003D00CF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0061001C-00E2-4CCE-B7A2-00C800E40099}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D47</xm:sqref>
+          <xm:sqref>D54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A9009C-00D1-4CD7-8ABB-007500D30075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00F90082-0007-406E-8F14-002C009300F6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D50</xm:sqref>
+          <xm:sqref>D57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00810065-00C2-4C91-9E5A-007500E60017}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00EB0067-0040-48CD-877D-00D300CC00FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D52</xm:sqref>
+          <xm:sqref>D59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EE0036-009A-4C1F-A04D-007200460008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0033007F-0009-4399-847F-0049007A00F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D62</xm:sqref>
+          <xm:sqref>D69</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F70017-007D-4C81-B9D5-00CE00C500D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0020001C-0070-4B2A-B7B4-0054004700ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G63</xm:sqref>
+          <xm:sqref>G70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007500D1-00FA-4B5E-A73B-005E008D0051}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{004B006A-0087-4350-8486-000500490003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G66</xm:sqref>
+          <xm:sqref>G73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001000F2-0012-4608-9EAF-00AD004600E0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0071000C-0091-4E7E-B52B-002A003E0054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -3903,7 +4089,7 @@
           </x14:formula2>
           <xm:sqref>A4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D70067-00DA-48FF-9F7E-00A300650059}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{004C00D8-00FF-455F-BEC7-00800056000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -3912,25 +4098,25 @@
           </x14:formula2>
           <xm:sqref>A3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00030017-002C-4FB2-A971-00150035009F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00A00091-0024-489C-8021-0008002C0047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D11:D12 D13:D20 D9</xm:sqref>
+          <xm:sqref>D11:D12 D13:D23 D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004F008D-00FD-406F-88C3-002B007500B9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00710009-007C-411D-B6FE-00110096006D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A11:A12 A13:A20 A9</xm:sqref>
+          <xm:sqref>A11:A12 A13:A23 A9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A6005C-00B3-4D4D-9324-00C1003A0043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D000A9-009F-4AC4-9C18-0093003300BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -3939,77 +4125,77 @@
           </x14:formula2>
           <xm:sqref>A5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007900EF-0085-49DA-8A5E-001E00000018}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{007000A1-004D-4D29-9C28-0075002900F5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D79</xm:sqref>
+          <xm:sqref>D86</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EA0070-00B1-4231-969E-0099000400BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{003B00B5-0072-49CD-831C-00E100A90079}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A79</xm:sqref>
+          <xm:sqref>A86</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DC00E5-0090-4399-AD73-0002009C0026}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00FD0097-0001-4143-9261-00F800C70008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D32</xm:sqref>
+          <xm:sqref>D36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007200BD-0085-415A-AE8F-002800A600CA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00BF00C9-00DF-46C9-A933-0035002A0034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A32</xm:sqref>
+          <xm:sqref>A36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001C00D8-007A-4961-9CD2-008A00DC0085}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{000400A1-00B4-4B8B-B5D8-0013003E0008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D78</xm:sqref>
+          <xm:sqref>D85</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0049009A-00F9-4622-8E71-00890071007E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00FC0066-00CF-49F4-9043-00190082005D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A78</xm:sqref>
+          <xm:sqref>A85</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F7000B-00C4-4D2C-96C1-00DF009C0095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{009400D6-00B9-4760-8E55-0022005E0096}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D23</xm:sqref>
+          <xm:sqref>D26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003D0037-00CC-49B8-AE5D-000E0033006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00F3006B-0056-49EA-9891-008D000B00E3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A23</xm:sqref>
+          <xm:sqref>A26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4039,7 +4225,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
@@ -4065,13 +4251,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -4113,13 +4299,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -4140,13 +4326,13 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -4166,13 +4352,13 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -4192,13 +4378,13 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -4218,13 +4404,13 @@
     </row>
     <row r="8" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -4244,13 +4430,13 @@
     </row>
     <row r="9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -4290,13 +4476,13 @@
     </row>
     <row r="11" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -4316,13 +4502,13 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -6178,25 +6364,25 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -6220,23 +6406,23 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="24" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-09-01 14-09</v>
+        <v xml:space="preserve">2022-09-28 16-44</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -6267,7 +6453,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1</v>
@@ -6276,22 +6462,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
@@ -6310,13 +6496,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
@@ -6341,13 +6527,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
@@ -6397,13 +6583,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
@@ -6428,13 +6614,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
@@ -6459,13 +6645,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
@@ -6490,13 +6676,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -6521,13 +6707,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -6577,13 +6763,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="34" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -6608,13 +6794,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="34" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -6639,13 +6825,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="34" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -6670,13 +6856,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="34" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -6701,13 +6887,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
@@ -6732,13 +6918,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
@@ -6788,13 +6974,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
@@ -6819,13 +7005,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="34" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
@@ -6850,13 +7036,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
@@ -6881,13 +7067,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="34" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
@@ -6912,13 +7098,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
@@ -6943,13 +7129,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
@@ -6999,13 +7185,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="34" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
@@ -7030,13 +7216,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="34" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
@@ -7061,13 +7247,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="34" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
@@ -7092,13 +7278,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
@@ -7123,13 +7309,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
@@ -7179,13 +7365,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="34" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
@@ -7210,13 +7396,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="34" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
@@ -7266,121 +7452,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B47" si="0">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B43" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -7391,26 +7577,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -7421,13 +7607,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="35" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D48" s="35"/>
       <c r="E48" s="35"/>
@@ -7452,13 +7638,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="35" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C49" s="35" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D49" s="35"/>
       <c r="E49" s="35"/>
@@ -7484,226 +7670,226 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B51" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C51" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B52" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C52" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B53" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C53" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B54" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C54" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B55" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C55" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="35" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C58" s="35" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="35" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="35" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="35" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="33" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="33" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C64" s="35" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="33" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="33" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B66" s="33" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C66" s="35" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="33" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B67" s="33" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B69" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C69" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B70" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C70" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B72" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C72" s="36" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B73" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C73" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B74" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C74" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Switch to use replacement_contact_id in the replace user forms
</commit_message>
<xml_diff>
--- a/config/default/forms/app/replace_user.xlsx
+++ b/config/default/forms/app/replace_user.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="299">
   <si>
     <t>type</t>
   </si>
@@ -531,10 +531,7 @@
     <t>/replace_user</t>
   </si>
   <si>
-    <t>original_contact_uuid</t>
-  </si>
-  <si>
-    <t>new_contact_uuid</t>
+    <t>replacement_contact_id</t>
   </si>
   <si>
     <t>${new_contact}</t>
@@ -1276,7 +1273,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{F68F2BEC-0C94-05D9-E827-15E919827533}"/>
+  <person displayName=" " id="{22E6871B-7AE3-8F3D-D05D-823DAFC52E6F}"/>
 </personList>
 </file>
 
@@ -1692,7 +1689,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="M1" personId="{F68F2BEC-0C94-05D9-E827-15E919827533}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
+  <threadedComment ref="M1" personId="{22E6871B-7AE3-8F3D-D05D-823DAFC52E6F}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
     <text xml:space="preserve">Comment:
 +marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
@@ -3963,41 +3960,17 @@
       <c r="G85" s="19"/>
       <c r="H85" s="18"/>
       <c r="I85" s="18" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
       <c r="J85" s="18"/>
       <c r="K85" s="19"/>
       <c r="L85" s="19"/>
       <c r="M85" s="19"/>
-      <c r="N85" s="18"/>
+      <c r="N85" s="18" t="s">
+        <v>158</v>
+      </c>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
-    </row>
-    <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B86" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C86" s="18"/>
-      <c r="D86" s="19"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="19"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="J86" s="18"/>
-      <c r="K86" s="19"/>
-      <c r="L86" s="19"/>
-      <c r="M86" s="19"/>
-      <c r="N86" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="O86" s="1"/>
-      <c r="P86" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -4007,8 +3980,8 @@
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="21" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0089006D-0001-4BE3-9625-004A00F4008B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="19" disablePrompts="0">
+        <x14:dataValidation xr:uid="{009200B1-00F8-4241-8AE5-00B2001300EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4017,7 +3990,7 @@
           </x14:formula2>
           <xm:sqref>D2:D8 D10 D24:D25 D35 D41:D53 D81:D82 D83:D84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007000BF-001F-431C-9A34-001200B2001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00ED0022-00DA-40CA-9BC8-001A00DD0087}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4026,7 +3999,7 @@
           </x14:formula2>
           <xm:sqref>A1:A2 A6:A8 A10 A24:A25 A35 A41:A53 A81:A82 A83:A84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0061001C-00E2-4CCE-B7A2-00C800E40099}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{007B00A4-0086-4067-A376-002800580025}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4035,7 +4008,7 @@
           </x14:formula2>
           <xm:sqref>D54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F90082-0007-406E-8F14-002C009300F6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00CD00CD-00CB-41DF-9B9F-009900CA0026}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4044,7 +4017,7 @@
           </x14:formula2>
           <xm:sqref>D57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EB0067-0040-48CD-877D-00D300CC00FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00FE00B3-00CA-4377-9958-0018007F00DF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4053,7 +4026,7 @@
           </x14:formula2>
           <xm:sqref>D59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0033007F-0009-4399-847F-0049007A00F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00CD005F-00CF-4BA7-9285-00AD00CD00A7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4062,7 +4035,7 @@
           </x14:formula2>
           <xm:sqref>D69</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0020001C-0070-4B2A-B7B4-0054004700ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0034000A-009F-450E-8DC7-00FB00870027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4071,7 +4044,7 @@
           </x14:formula2>
           <xm:sqref>G70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004B006A-0087-4350-8486-000500490003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{004D0015-0080-486E-A727-00B300A30069}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4080,7 +4053,7 @@
           </x14:formula2>
           <xm:sqref>G73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0071000C-0091-4E7E-B52B-002A003E0054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{009F0075-0021-4AF8-8B71-006E002E00FF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4089,7 +4062,7 @@
           </x14:formula2>
           <xm:sqref>A4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004C00D8-00FF-455F-BEC7-00800056000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00190062-0070-41F2-B39B-0011002200EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4098,7 +4071,7 @@
           </x14:formula2>
           <xm:sqref>A3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A00091-0024-489C-8021-0008002C0047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0065003A-00B2-4CFC-90B3-00A8005D00F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4107,7 +4080,7 @@
           </x14:formula2>
           <xm:sqref>D11:D12 D13:D23 D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00710009-007C-411D-B6FE-00110096006D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{006D0011-00C3-426D-8C57-00AD00ED0055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4116,7 +4089,7 @@
           </x14:formula2>
           <xm:sqref>A11:A12 A13:A23 A9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D000A9-009F-4AC4-9C18-0093003300BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{008E0088-0059-4CA0-AD0B-00E4007F00F1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4125,25 +4098,25 @@
           </x14:formula2>
           <xm:sqref>A5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007000A1-004D-4D29-9C28-0075002900F5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00020087-0086-480A-85A7-0023009A007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D86</xm:sqref>
+          <xm:sqref>D85</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003B00B5-0072-49CD-831C-00E100A90079}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00360045-0043-47E1-A50B-0008002F00E3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A86</xm:sqref>
+          <xm:sqref>A85</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FD0097-0001-4143-9261-00F800C70008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00A7000B-000B-45B6-BA5C-00FA00F30030}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4152,7 +4125,7 @@
           </x14:formula2>
           <xm:sqref>D36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00BF00C9-00DF-46C9-A933-0035002A0034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00C400B8-0018-4C48-AED3-009000EF008A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4161,25 +4134,7 @@
           </x14:formula2>
           <xm:sqref>A36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000400A1-00B4-4B8B-B5D8-0013003E0008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
-          <x14:formula1>
-            <xm:f>"yes,no"</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>D85</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FC0066-00CF-49F4-9043-00190082005D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
-          <x14:formula1>
-            <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>A85</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009400D6-00B9-4760-8E55-0022005E0096}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{004500BF-00BA-4461-B741-003200DB00B2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4188,7 +4143,7 @@
           </x14:formula2>
           <xm:sqref>D26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F3006B-0056-49EA-9891-008D000B00E3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{003B0001-006A-460B-A0F3-002500C800E9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4225,7 +4180,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
@@ -4251,13 +4206,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -4299,13 +4254,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>165</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>166</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -4326,13 +4281,13 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>167</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>168</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -4352,13 +4307,13 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -4378,13 +4333,13 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -4404,13 +4359,13 @@
     </row>
     <row r="8" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>173</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -4430,13 +4385,13 @@
     </row>
     <row r="9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>176</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -4476,13 +4431,13 @@
     </row>
     <row r="11" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="C11" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>179</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -4502,13 +4457,13 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>180</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>181</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -6364,25 +6319,25 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -6406,23 +6361,23 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>189</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>190</v>
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-09-28 16-44</v>
+        <v xml:space="preserve">2022-09-28 16-51</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="G2" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -6453,7 +6408,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1</v>
@@ -6462,22 +6417,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="32" t="s">
         <v>198</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>199</v>
       </c>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
@@ -6496,13 +6451,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="C2" s="34" t="s">
         <v>201</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>202</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
@@ -6527,13 +6482,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>203</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>204</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
@@ -6583,13 +6538,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="C5" s="34" t="s">
         <v>206</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>207</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
@@ -6614,13 +6569,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="34" t="s">
         <v>208</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>209</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
@@ -6645,13 +6600,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>210</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>211</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
@@ -6676,13 +6631,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B8" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>213</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -6707,13 +6662,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B9" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>214</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>215</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -6763,13 +6718,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="C11" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>218</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -6794,13 +6749,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>219</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>220</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -6825,13 +6780,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B13" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" s="34" t="s">
         <v>221</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>222</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -6856,13 +6811,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" s="34" t="s">
         <v>223</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>224</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -6887,13 +6842,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="34" t="s">
         <v>225</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>226</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
@@ -6918,13 +6873,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B16" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="34" t="s">
         <v>227</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>228</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
@@ -6974,13 +6929,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B18" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="C18" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>218</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
@@ -7005,13 +6960,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B19" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>219</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>220</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
@@ -7036,13 +6991,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B20" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>221</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>222</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
@@ -7067,13 +7022,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B21" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C21" s="34" t="s">
         <v>223</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>224</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
@@ -7098,13 +7053,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B22" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="C22" s="34" t="s">
         <v>227</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>228</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
@@ -7129,13 +7084,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="B23" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="C23" s="34" t="s">
         <v>230</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>231</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
@@ -7185,13 +7140,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="C25" s="34" t="s">
         <v>233</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>234</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
@@ -7216,13 +7171,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B26" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="34" t="s">
         <v>235</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>236</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
@@ -7247,13 +7202,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B27" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" s="34" t="s">
         <v>237</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>238</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
@@ -7278,13 +7233,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B28" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" s="34" t="s">
         <v>239</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>240</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
@@ -7309,13 +7264,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B29" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="34" t="s">
         <v>175</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>176</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
@@ -7365,13 +7320,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="B31" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="B31" s="34" t="s">
-        <v>242</v>
-      </c>
       <c r="C31" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
@@ -7396,13 +7351,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
@@ -7452,121 +7407,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B47" si="0">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B43" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" t="s">
         <v>175</v>
-      </c>
-      <c r="C43" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -7577,26 +7532,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -7607,13 +7562,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="B48" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="C48" s="35" t="s">
         <v>258</v>
-      </c>
-      <c r="C48" s="35" t="s">
-        <v>259</v>
       </c>
       <c r="D48" s="35"/>
       <c r="E48" s="35"/>
@@ -7638,13 +7593,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B49" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="C49" s="35" t="s">
         <v>260</v>
-      </c>
-      <c r="C49" s="35" t="s">
-        <v>261</v>
       </c>
       <c r="D49" s="35"/>
       <c r="E49" s="35"/>
@@ -7670,226 +7625,226 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
+        <v>261</v>
+      </c>
+      <c r="B51" t="s">
         <v>262</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>263</v>
-      </c>
-      <c r="C51" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B52" t="s">
+        <v>264</v>
+      </c>
+      <c r="C52" t="s">
         <v>265</v>
-      </c>
-      <c r="C52" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B53" t="s">
+        <v>266</v>
+      </c>
+      <c r="C53" t="s">
         <v>267</v>
-      </c>
-      <c r="C53" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B54" t="s">
+        <v>268</v>
+      </c>
+      <c r="C54" t="s">
         <v>269</v>
-      </c>
-      <c r="C54" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B55" t="s">
+        <v>270</v>
+      </c>
+      <c r="C55" t="s">
         <v>271</v>
-      </c>
-      <c r="C55" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B56" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" t="s">
         <v>175</v>
-      </c>
-      <c r="C56" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="B58" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="C58" s="35" t="s">
         <v>274</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="35" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B59" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C59" s="35" t="s">
         <v>276</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="35" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B60" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="C60" s="35" t="s">
         <v>278</v>
-      </c>
-      <c r="C60" s="35" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="35" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B61" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="35" t="s">
         <v>175</v>
-      </c>
-      <c r="C61" s="35" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="B63" s="33" t="s">
         <v>280</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="C63" s="35" t="s">
         <v>281</v>
-      </c>
-      <c r="C63" s="35" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B64" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="C64" s="35" t="s">
         <v>283</v>
-      </c>
-      <c r="C64" s="35" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B65" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="C65" s="35" t="s">
         <v>285</v>
-      </c>
-      <c r="C65" s="35" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B66" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="C66" s="35" t="s">
         <v>287</v>
-      </c>
-      <c r="C66" s="35" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B67" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="C67" s="35" t="s">
         <v>289</v>
-      </c>
-      <c r="C67" s="35" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
+        <v>290</v>
+      </c>
+      <c r="B69" t="s">
         <v>291</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>292</v>
-      </c>
-      <c r="C69" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B70" t="s">
+        <v>293</v>
+      </c>
+      <c r="C70" t="s">
         <v>294</v>
-      </c>
-      <c r="C70" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
+        <v>295</v>
+      </c>
+      <c r="B72" t="s">
         <v>296</v>
       </c>
-      <c r="B72" t="s">
-        <v>297</v>
-      </c>
       <c r="C72" s="36" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B73" t="s">
+        <v>297</v>
+      </c>
+      <c r="C73" t="s">
         <v>298</v>
-      </c>
-      <c r="C73" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B74" t="s">
+        <v>174</v>
+      </c>
+      <c r="C74" t="s">
         <v>175</v>
-      </c>
-      <c r="C74" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add warning outro to replace_user
</commit_message>
<xml_diff>
--- a/config/default/forms/app/replace_user.xlsx
+++ b/config/default/forms/app/replace_user.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="305">
   <si>
     <t>type</t>
   </si>
@@ -535,6 +535,27 @@
   </si>
   <si>
     <t>${new_contact}</t>
+  </si>
+  <si>
+    <t>new_contact_name</t>
+  </si>
+  <si>
+    <t>../new_contact/name</t>
+  </si>
+  <si>
+    <t>new_contact_phone</t>
+  </si>
+  <si>
+    <t>../new_contact/phone</t>
+  </si>
+  <si>
+    <t>outro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submitting this form will cause the current user to be *automatically logged after the next sync.*
+This could happen immediately if you are currently connected to the internet.
+After the current user is logged out, a SMS message will be sent to **${new_contact_phone}** containing a login link. Open that link to login as **${new_contact_name}**.
+Please contact your administrator if you do not receive a login link.</t>
   </si>
   <si>
     <t>list_name</t>
@@ -1273,7 +1294,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{22E6871B-7AE3-8F3D-D05D-823DAFC52E6F}"/>
+  <person displayName=" " id="{7371A0CD-B85C-02A2-F92F-C7F4F045717A}"/>
 </personList>
 </file>
 
@@ -1689,7 +1710,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="M1" personId="{22E6871B-7AE3-8F3D-D05D-823DAFC52E6F}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
+  <threadedComment ref="M1" personId="{7371A0CD-B85C-02A2-F92F-C7F4F045717A}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
     <text xml:space="preserve">Comment:
 +marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
@@ -3929,20 +3950,28 @@
       <c r="P83" s="1"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="10"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="10"/>
-      <c r="I84" s="10"/>
-      <c r="J84" s="10"/>
-      <c r="K84" s="1"/>
-      <c r="L84" s="1"/>
-      <c r="M84" s="1"/>
-      <c r="N84" s="1"/>
+      <c r="A84" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B84" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="18"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="J84" s="18"/>
+      <c r="K84" s="19"/>
+      <c r="L84" s="19"/>
+      <c r="M84" s="19"/>
+      <c r="N84" s="18" t="s">
+        <v>158</v>
+      </c>
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
     </row>
@@ -3951,7 +3980,7 @@
         <v>44</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C85" s="18"/>
       <c r="D85" s="19"/>
@@ -3960,18 +3989,267 @@
       <c r="G85" s="19"/>
       <c r="H85" s="18"/>
       <c r="I85" s="18" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J85" s="18"/>
       <c r="K85" s="19"/>
       <c r="L85" s="19"/>
       <c r="M85" s="19"/>
-      <c r="N85" s="18" t="s">
-        <v>158</v>
-      </c>
+      <c r="N85" s="18"/>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
     </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C86" s="18"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="J86" s="18"/>
+      <c r="K86" s="19"/>
+      <c r="L86" s="19"/>
+      <c r="M86" s="19"/>
+      <c r="N86" s="18"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+    </row>
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="A87" s="10"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="10"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+    </row>
+    <row r="88" ht="15.75" customHeight="1">
+      <c r="A88" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G88" s="19"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+      <c r="J88" s="18"/>
+      <c r="K88" s="19"/>
+      <c r="L88" s="19"/>
+      <c r="M88" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="N88" s="19"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+    </row>
+    <row r="89" ht="15.75" customHeight="1">
+      <c r="A89" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G89" s="19"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="19"/>
+      <c r="L89" s="19"/>
+      <c r="M89" s="19"/>
+      <c r="N89" s="19"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+    </row>
+    <row r="90" ht="15.75" customHeight="1">
+      <c r="A90" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="19"/>
+      <c r="L90" s="19"/>
+      <c r="M90" s="19"/>
+      <c r="N90" s="19"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+    </row>
+    <row r="91" ht="15.75" customHeight="1">
+      <c r="A91" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C91" s="18"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="19"/>
+      <c r="L91" s="19"/>
+      <c r="M91" s="19"/>
+      <c r="N91" s="19"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+    </row>
+    <row r="92" ht="15.75" customHeight="1">
+      <c r="A92" s="10"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+    </row>
+    <row r="93" ht="15.75" customHeight="1">
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+    </row>
+    <row r="94" ht="15.75" customHeight="1">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+    </row>
+    <row r="95" ht="15.75" customHeight="1">
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+    </row>
+    <row r="96" ht="15.75" customHeight="1">
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="J96" s="10"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+    </row>
+    <row r="97" ht="15.75" customHeight="1">
+      <c r="A97" s="10"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+    </row>
+    <row r="98" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3980,26 +4258,26 @@
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="19" disablePrompts="0">
-        <x14:dataValidation xr:uid="{009200B1-00F8-4241-8AE5-00B2001300EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="21" disablePrompts="0">
+        <x14:dataValidation xr:uid="{0092009C-005C-4694-9F2C-00F6002300AC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D2:D8 D10 D24:D25 D35 D41:D53 D81:D82 D83:D84</xm:sqref>
+          <xm:sqref>D2:D8 D10 D24:D25 D35 D41:D53 D81:D82 D83 D87</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00ED0022-00DA-40CA-9BC8-001A00DD0087}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{000E009D-0009-41C4-B9A8-0088004700ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A1:A2 A6:A8 A10 A24:A25 A35 A41:A53 A81:A82 A83:A84</xm:sqref>
+          <xm:sqref>A1:A2 A6:A8 A10 A24:A25 A35 A41:A53 A81:A82 A83 A87</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007B00A4-0086-4067-A376-002800580025}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00BE007E-0010-467F-82DF-0019009700B5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4008,7 +4286,7 @@
           </x14:formula2>
           <xm:sqref>D54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CD00CD-00CB-41DF-9B9F-009900CA0026}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{008F00FA-00D9-41E3-9764-00EA004D00BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4017,7 +4295,7 @@
           </x14:formula2>
           <xm:sqref>D57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FE00B3-00CA-4377-9958-0018007F00DF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00390024-00E4-4D4C-9D29-004800F000FD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4026,7 +4304,7 @@
           </x14:formula2>
           <xm:sqref>D59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CD005F-00CF-4BA7-9285-00AD00CD00A7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{006B00FE-00EE-43B6-A20D-005100AC002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4035,7 +4313,7 @@
           </x14:formula2>
           <xm:sqref>D69</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0034000A-009F-450E-8DC7-00FB00870027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00E700C3-000E-4328-9495-009000180085}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4044,7 +4322,7 @@
           </x14:formula2>
           <xm:sqref>G70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004D0015-0080-486E-A727-00B300A30069}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{008300CE-0080-4886-8A07-008600AD005B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4053,7 +4331,7 @@
           </x14:formula2>
           <xm:sqref>G73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009F0075-0021-4AF8-8B71-006E002E00FF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{002600F5-0039-4DFA-B8EF-001500160070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4062,7 +4340,7 @@
           </x14:formula2>
           <xm:sqref>A4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00190062-0070-41F2-B39B-0011002200EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00BA0006-0014-4034-9F12-0016004600E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4071,7 +4349,7 @@
           </x14:formula2>
           <xm:sqref>A3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0065003A-00B2-4CFC-90B3-00A8005D00F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0000003B-0081-4AA5-A0ED-00BE0096002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4080,7 +4358,7 @@
           </x14:formula2>
           <xm:sqref>D11:D12 D13:D23 D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006D0011-00C3-426D-8C57-00AD00ED0055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00B10038-000E-4041-8AC5-003F00C1002E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4089,7 +4367,7 @@
           </x14:formula2>
           <xm:sqref>A11:A12 A13:A23 A9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008E0088-0059-4CA0-AD0B-00E4007F00F1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{006C0045-0063-4886-A5E8-006D004D0024}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4098,25 +4376,25 @@
           </x14:formula2>
           <xm:sqref>A5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00020087-0086-480A-85A7-0023009A007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{009C0098-000E-456F-9988-0007005B00A9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D85</xm:sqref>
+          <xm:sqref>D84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00360045-0043-47E1-A50B-0008002F00E3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0006004A-002C-45D8-84A6-00F0005600A4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A85</xm:sqref>
+          <xm:sqref>A84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A7000B-000B-45B6-BA5C-00FA00F30030}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00BC00E0-00F4-4397-BF6E-00BB008900ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4125,7 +4403,7 @@
           </x14:formula2>
           <xm:sqref>D36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C400B8-0018-4C48-AED3-009000EF008A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{005A0034-0020-45B1-B3A6-00DB004E0041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4134,7 +4412,7 @@
           </x14:formula2>
           <xm:sqref>A36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004500BF-00BA-4461-B741-003200DB00B2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00EE0086-00D0-4149-98B8-0038003B007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4143,7 +4421,7 @@
           </x14:formula2>
           <xm:sqref>D26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003B0001-006A-460B-A0F3-002500C800E9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00900005-0081-4FA3-8A8C-003700770027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4151,6 +4429,24 @@
             <xm:f>0</xm:f>
           </x14:formula2>
           <xm:sqref>A26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00F6005E-00A0-4DB5-993C-00BF00C1000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+          <x14:formula1>
+            <xm:f>"yes,no"</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>D88</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D400F9-00F2-4559-84E2-00BE003900EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+          <x14:formula1>
+            <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>A88</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4180,7 +4476,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
@@ -4206,13 +4502,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -4254,13 +4550,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -4281,13 +4577,13 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -4307,13 +4603,13 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -4333,13 +4629,13 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -4359,13 +4655,13 @@
     </row>
     <row r="8" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -4385,13 +4681,13 @@
     </row>
     <row r="9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -4431,13 +4727,13 @@
     </row>
     <row r="11" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -4457,13 +4753,13 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -6319,25 +6615,25 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -6361,23 +6657,23 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="24" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-09-28 16-51</v>
+        <v xml:space="preserve">2022-09-28 21-40</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -6408,7 +6704,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1</v>
@@ -6417,22 +6713,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
@@ -6451,13 +6747,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
@@ -6482,13 +6778,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
@@ -6538,13 +6834,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
@@ -6569,13 +6865,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
@@ -6600,13 +6896,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
@@ -6631,13 +6927,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -6662,13 +6958,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -6718,13 +7014,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="34" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -6749,13 +7045,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="34" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -6780,13 +7076,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="34" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -6811,13 +7107,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="34" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -6842,13 +7138,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
@@ -6873,13 +7169,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
@@ -6929,13 +7225,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
@@ -6960,13 +7256,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="34" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
@@ -6991,13 +7287,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
@@ -7022,13 +7318,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="B21" s="34" t="s">
-        <v>222</v>
-      </c>
       <c r="C21" s="34" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
@@ -7053,13 +7349,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
@@ -7084,13 +7380,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
@@ -7140,13 +7436,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="34" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
@@ -7171,13 +7467,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="34" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
@@ -7202,13 +7498,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="34" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
@@ -7233,13 +7529,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
@@ -7264,13 +7560,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
@@ -7320,13 +7616,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="34" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
@@ -7351,13 +7647,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="34" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
@@ -7407,121 +7703,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B47" si="0">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B43" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C43" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -7532,26 +7828,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -7562,13 +7858,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="35" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="D48" s="35"/>
       <c r="E48" s="35"/>
@@ -7593,13 +7889,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="35" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C49" s="35" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D49" s="35"/>
       <c r="E49" s="35"/>
@@ -7625,226 +7921,226 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B51" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C51" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B52" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C52" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B53" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C53" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B54" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C54" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B55" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C55" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B56" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C56" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="35" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C58" s="35" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="35" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="35" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="35" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="33" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="33" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="C64" s="35" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="33" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="33" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B66" s="33" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C66" s="35" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="33" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B67" s="33" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B69" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C69" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B70" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="C70" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B72" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C72" s="36" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B73" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="C73" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B74" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C74" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add constraints to `replace_user` form visibility (#7827)
Co-authored-by: Joshua Kuestersteffen <jkuester@kuester7.com>
</commit_message>
<xml_diff>
--- a/config/default/forms/app/replace_user.xlsx
+++ b/config/default/forms/app/replace_user.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="305">
   <si>
     <t>type</t>
   </si>
@@ -176,10 +176,13 @@
     <t>parent</t>
   </si>
   <si>
-    <t xml:space="preserve">Household ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area ID</t>
+    <t xml:space="preserve">Parent 1 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent 2 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent 3 ID</t>
   </si>
   <si>
     <t>calculate</t>
@@ -194,16 +197,22 @@
     <t>../inputs/contact/_id</t>
   </si>
   <si>
-    <t>contact_area_id</t>
+    <t>parent_1_id</t>
   </si>
   <si>
     <t>../inputs/contact/parent/_id</t>
   </si>
   <si>
-    <t>contact_facility_id</t>
+    <t>parent_2_id</t>
   </si>
   <si>
     <t>../inputs/contact/parent/parent/_id</t>
+  </si>
+  <si>
+    <t>parent_3_id</t>
+  </si>
+  <si>
+    <t>../inputs/contact/parent/parent/parent/_id</t>
   </si>
   <si>
     <t>user_phone</t>
@@ -279,16 +288,19 @@
     <t xml:space="preserve">New User</t>
   </si>
   <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>${contact_area_id}</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>${contact_facility_id}</t>
+    <t>${parent_1_id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${parent_2_id} != ''</t>
+  </si>
+  <si>
+    <t>${parent_2_id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${parent_3_id} != ''</t>
+  </si>
+  <si>
+    <t>${parent_3_id}</t>
   </si>
   <si>
     <t>Type</t>
@@ -453,7 +465,7 @@
     <t>phone_read_only</t>
   </si>
   <si>
-    <t>boolean(${user_phone})</t>
+    <t xml:space="preserve">${user_phone} != ''</t>
   </si>
   <si>
     <t>${user_phone}</t>
@@ -468,7 +480,7 @@
     <t>new_phone</t>
   </si>
   <si>
-    <t>not(boolean(${user_phone}))</t>
+    <t xml:space="preserve">${user_phone} = ''</t>
   </si>
   <si>
     <t xml:space="preserve">Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +254712345678</t>
@@ -519,13 +531,31 @@
     <t>/replace_user</t>
   </si>
   <si>
-    <t>original_contact_uuid</t>
-  </si>
-  <si>
-    <t>new_contact_uuid</t>
+    <t>replacement_contact_id</t>
   </si>
   <si>
     <t>${new_contact}</t>
+  </si>
+  <si>
+    <t>new_contact_name</t>
+  </si>
+  <si>
+    <t>../new_contact/name</t>
+  </si>
+  <si>
+    <t>new_contact_phone</t>
+  </si>
+  <si>
+    <t>../new_contact/phone</t>
+  </si>
+  <si>
+    <t>outro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submitting this form will cause the current user to be *automatically logged after the next sync.*
+This could happen immediately if you are currently connected to the internet.
+After the current user is logged out, a SMS message will be sent to **${new_contact_phone}** containing a login link. Open that link to login as **${new_contact_name}**.
+Please contact your administrator if you do not receive a login link.</t>
   </si>
   <si>
     <t>list_name</t>
@@ -1264,7 +1294,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{5C008D89-1249-1821-A035-20B9C9B30380}"/>
+  <person displayName=" " id="{7371A0CD-B85C-02A2-F92F-C7F4F045717A}"/>
 </personList>
 </file>
 
@@ -1680,7 +1710,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="M1" personId="{5C008D89-1249-1821-A035-20B9C9B30380}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
+  <threadedComment ref="M1" personId="{7371A0CD-B85C-02A2-F92F-C7F4F045717A}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
     <text xml:space="preserve">Comment:
 +marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
@@ -2151,9 +2181,7 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -2195,12 +2223,14 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -2219,12 +2249,14 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -2246,7 +2278,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -2270,7 +2302,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -2284,118 +2316,118 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="A22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="14"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+      <c r="A23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="A24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J25" s="14"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="14"/>
+        <v>45</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="15" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="16"/>
@@ -2407,10 +2439,10 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -2419,7 +2451,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="16"/>
@@ -2428,42 +2460,26 @@
       <c r="N27" s="15"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
-      <c r="AF27" s="1"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
       <c r="I28" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="1"/>
@@ -2471,23 +2487,23 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="14"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="1"/>
@@ -2495,233 +2511,251 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="14"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" ht="15">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="14"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-    </row>
-    <row r="32" ht="15">
-      <c r="A32" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G32" s="19"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="N32" s="19"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
+    <row r="35" ht="15">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
     <row r="36" ht="15">
       <c r="A36" s="17" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="18"/>
+        <v>64</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+      <c r="F36" s="19" t="s">
+        <v>65</v>
+      </c>
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
       <c r="J36" s="18"/>
       <c r="K36" s="19"/>
       <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
+      <c r="M36" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="N36" s="19"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" ht="15">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
+    <row r="37" ht="12.75" customHeight="1">
+      <c r="A37" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="19"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
-      <c r="F38" s="19" t="s">
-        <v>18</v>
-      </c>
+      <c r="F38" s="19"/>
       <c r="G38" s="19"/>
       <c r="H38" s="18"/>
       <c r="I38" s="19"/>
       <c r="J38" s="18"/>
       <c r="K38" s="19"/>
       <c r="L38" s="19"/>
-      <c r="M38" s="19" t="s">
-        <v>63</v>
-      </c>
+      <c r="M38" s="19"/>
       <c r="N38" s="19"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="19" t="s">
-        <v>19</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="18"/>
       <c r="I39" s="19"/>
@@ -2733,24 +2767,20 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" ht="15">
       <c r="A40" s="17" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>75</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C40" s="18"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
       <c r="H40" s="18"/>
-      <c r="I40" s="19" t="s">
-        <v>76</v>
-      </c>
+      <c r="I40" s="19"/>
       <c r="J40" s="18"/>
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
@@ -2759,69 +2789,67 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="19"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
+    <row r="41" ht="15">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
+      <c r="F42" s="19" t="s">
+        <v>18</v>
+      </c>
       <c r="G42" s="19"/>
       <c r="H42" s="18"/>
-      <c r="I42" s="19" t="s">
-        <v>78</v>
-      </c>
+      <c r="I42" s="19"/>
       <c r="J42" s="18"/>
       <c r="K42" s="19"/>
       <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
+      <c r="M42" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="N42" s="19"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="18"/>
+      <c r="C43" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="D43" s="19"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="19"/>
+      <c r="F43" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="G43" s="19"/>
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
@@ -2835,18 +2863,22 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="17" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="18"/>
+        <v>35</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="D44" s="19"/>
-      <c r="E44" s="18"/>
+      <c r="E44" s="19"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
       <c r="H44" s="18"/>
-      <c r="I44" s="19"/>
+      <c r="I44" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="J44" s="18"/>
       <c r="K44" s="19"/>
       <c r="L44" s="19"/>
@@ -2857,22 +2889,24 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C45" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="E45" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
+      <c r="F45" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="G45" s="19"/>
       <c r="H45" s="18"/>
-      <c r="I45" s="20" t="s">
-        <v>80</v>
-      </c>
+      <c r="I45" s="19"/>
       <c r="J45" s="18"/>
       <c r="K45" s="19"/>
       <c r="L45" s="19"/>
@@ -2883,22 +2917,22 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="17" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>72</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
       <c r="H46" s="18"/>
-      <c r="I46" s="19"/>
+      <c r="I46" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="J46" s="18"/>
       <c r="K46" s="19"/>
       <c r="L46" s="19"/>
@@ -2909,27 +2943,23 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="17" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
+      <c r="E47" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="F47" s="19"/>
-      <c r="G47" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>85</v>
-      </c>
+      <c r="G47" s="19"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="19"/>
-      <c r="J47" s="18" t="s">
-        <v>86</v>
-      </c>
+      <c r="J47" s="18"/>
       <c r="K47" s="19"/>
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
@@ -2939,21 +2969,21 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="19" t="s">
-        <v>72</v>
-      </c>
+      <c r="D48" s="19"/>
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
       <c r="H48" s="18"/>
       <c r="I48" s="19" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J48" s="18"/>
       <c r="K48" s="19"/>
@@ -2965,10 +2995,10 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="17" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="19"/>
@@ -2976,9 +3006,7 @@
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
       <c r="H49" s="18"/>
-      <c r="I49" s="19" t="s">
-        <v>90</v>
-      </c>
+      <c r="I49" s="19"/>
       <c r="J49" s="18"/>
       <c r="K49" s="19"/>
       <c r="L49" s="19"/>
@@ -2989,16 +3017,14 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="17" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>16</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C50" s="18"/>
       <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
+      <c r="E50" s="18"/>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
       <c r="H50" s="18"/>
@@ -3013,31 +3039,19 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="17" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>95</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="18"/>
       <c r="F51" s="19"/>
-      <c r="G51" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>97</v>
-      </c>
+      <c r="G51" s="19"/>
+      <c r="H51" s="18"/>
       <c r="I51" s="19"/>
-      <c r="J51" s="18" t="s">
-        <v>98</v>
-      </c>
+      <c r="J51" s="18"/>
       <c r="K51" s="19"/>
       <c r="L51" s="19"/>
       <c r="M51" s="19"/>
@@ -3047,22 +3061,22 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="17" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D52" s="19"/>
-      <c r="E52" s="19" t="s">
-        <v>101</v>
-      </c>
+      <c r="E52" s="19"/>
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
       <c r="H52" s="18"/>
-      <c r="I52" s="19"/>
+      <c r="I52" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="J52" s="18"/>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
@@ -3073,27 +3087,21 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>101</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E53" s="19"/>
       <c r="F53" s="19"/>
-      <c r="G53" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="H53" s="18" t="s">
-        <v>106</v>
-      </c>
+      <c r="G53" s="19"/>
+      <c r="H53" s="18"/>
       <c r="I53" s="19"/>
       <c r="J53" s="18"/>
       <c r="K53" s="19"/>
@@ -3105,27 +3113,27 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="17" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D54" s="19"/>
-      <c r="E54" s="19" t="s">
-        <v>101</v>
-      </c>
+      <c r="E54" s="19"/>
       <c r="F54" s="19"/>
       <c r="G54" s="19" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="I54" s="19"/>
-      <c r="J54" s="18"/>
+      <c r="J54" s="18" t="s">
+        <v>90</v>
+      </c>
       <c r="K54" s="19"/>
       <c r="L54" s="19"/>
       <c r="M54" s="19"/>
@@ -3135,22 +3143,22 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="17" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="19"/>
+        <v>91</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="E55" s="19"/>
-      <c r="F55" s="19" t="s">
-        <v>113</v>
-      </c>
+      <c r="F55" s="19"/>
       <c r="G55" s="19"/>
       <c r="H55" s="18"/>
-      <c r="I55" s="19"/>
+      <c r="I55" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="J55" s="18"/>
       <c r="K55" s="19"/>
       <c r="L55" s="19"/>
@@ -3161,10 +3169,10 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="19"/>
@@ -3173,7 +3181,7 @@
       <c r="G56" s="19"/>
       <c r="H56" s="18"/>
       <c r="I56" s="19" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="J56" s="18"/>
       <c r="K56" s="19"/>
@@ -3185,20 +3193,20 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C57" s="18"/>
+        <v>95</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="D57" s="19"/>
       <c r="E57" s="19"/>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
       <c r="H57" s="18"/>
-      <c r="I57" s="19" t="s">
-        <v>117</v>
-      </c>
+      <c r="I57" s="19"/>
       <c r="J57" s="18"/>
       <c r="K57" s="19"/>
       <c r="L57" s="19"/>
@@ -3209,21 +3217,31 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="17" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="J58" s="18"/>
+      <c r="G58" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I58" s="19"/>
+      <c r="J58" s="18" t="s">
+        <v>102</v>
+      </c>
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
       <c r="M58" s="19"/>
@@ -3233,20 +3251,22 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="17" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="18"/>
+        <v>103</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
+      <c r="E59" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
       <c r="H59" s="18"/>
-      <c r="I59" s="18" t="s">
-        <v>121</v>
-      </c>
+      <c r="I59" s="19"/>
       <c r="J59" s="18"/>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
@@ -3257,20 +3277,28 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="17" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
+        <v>107</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="19" t="s">
-        <v>123</v>
-      </c>
+      <c r="G60" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="I60" s="19"/>
       <c r="J60" s="18"/>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
@@ -3281,21 +3309,25 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="17" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="19" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="18"/>
+      <c r="G61" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="I61" s="19"/>
       <c r="J61" s="18"/>
       <c r="K61" s="19"/>
@@ -3307,15 +3339,19 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="18"/>
+        <v>116</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
+      <c r="F62" s="19" t="s">
+        <v>117</v>
+      </c>
       <c r="G62" s="19"/>
       <c r="H62" s="18"/>
       <c r="I62" s="19"/>
@@ -3329,24 +3365,20 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>72</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C63" s="18"/>
+      <c r="D63" s="19"/>
       <c r="E63" s="19"/>
-      <c r="F63" s="19" t="s">
-        <v>113</v>
-      </c>
+      <c r="F63" s="19"/>
       <c r="G63" s="19"/>
       <c r="H63" s="18"/>
-      <c r="I63" s="19"/>
+      <c r="I63" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="J63" s="18"/>
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
@@ -3357,31 +3389,23 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="17" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>31</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C64" s="18"/>
       <c r="D64" s="19"/>
-      <c r="E64" s="19" t="s">
-        <v>131</v>
-      </c>
+      <c r="E64" s="19"/>
       <c r="F64" s="19"/>
       <c r="G64" s="19"/>
       <c r="H64" s="18"/>
       <c r="I64" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="J64" s="18" t="s">
-        <v>133</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="J64" s="18"/>
       <c r="K64" s="19"/>
-      <c r="L64" s="19" t="s">
-        <v>72</v>
-      </c>
+      <c r="L64" s="19"/>
       <c r="M64" s="19"/>
       <c r="N64" s="19"/>
       <c r="O64" s="1"/>
@@ -3389,28 +3413,20 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D65" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>136</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C65" s="18"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
       <c r="F65" s="19"/>
-      <c r="G65" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H65" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="I65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="19" t="s">
+        <v>123</v>
+      </c>
       <c r="J65" s="18"/>
       <c r="K65" s="19"/>
       <c r="L65" s="19"/>
@@ -3421,21 +3437,19 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>31</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C66" s="18"/>
       <c r="D66" s="19"/>
       <c r="E66" s="19"/>
       <c r="F66" s="19"/>
       <c r="G66" s="19"/>
       <c r="H66" s="18"/>
-      <c r="I66" s="19" t="s">
-        <v>138</v>
+      <c r="I66" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="J66" s="18"/>
       <c r="K66" s="19"/>
@@ -3447,24 +3461,20 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="17" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>140</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C67" s="18"/>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
       <c r="F67" s="19"/>
-      <c r="G67" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H67" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="I67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="19" t="s">
+        <v>127</v>
+      </c>
       <c r="J67" s="18"/>
       <c r="K67" s="19"/>
       <c r="L67" s="19"/>
@@ -3472,81 +3482,41 @@
       <c r="N67" s="19"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1"/>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="1"/>
-      <c r="AD67" s="1"/>
-      <c r="AE67" s="1"/>
-      <c r="AF67" s="1"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="17" t="s">
-        <v>141</v>
+        <v>67</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19" t="s">
-        <v>142</v>
-      </c>
+      <c r="E68" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="19"/>
       <c r="G68" s="19"/>
       <c r="H68" s="18"/>
-      <c r="I68" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="J68" s="18" t="s">
-        <v>133</v>
-      </c>
+      <c r="I68" s="19"/>
+      <c r="J68" s="18"/>
       <c r="K68" s="19"/>
-      <c r="L68" s="19" t="s">
-        <v>72</v>
-      </c>
+      <c r="L68" s="19"/>
       <c r="M68" s="19"/>
       <c r="N68" s="19"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-      <c r="Z68" s="1"/>
-      <c r="AA68" s="1"/>
-      <c r="AB68" s="1"/>
-      <c r="AC68" s="1"/>
-      <c r="AD68" s="1"/>
-      <c r="AE68" s="1"/>
-      <c r="AF68" s="1"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>145</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C69" s="18"/>
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
       <c r="F69" s="19"/>
@@ -3560,37 +3530,23 @@
       <c r="N69" s="19"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="1"/>
-      <c r="V69" s="1"/>
-      <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-      <c r="AA69" s="1"/>
-      <c r="AB69" s="1"/>
-      <c r="AC69" s="1"/>
-      <c r="AD69" s="1"/>
-      <c r="AE69" s="1"/>
-      <c r="AF69" s="1"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="17" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="19"/>
+        <v>132</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="E70" s="19"/>
       <c r="F70" s="19" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="G70" s="19"/>
       <c r="H70" s="18"/>
@@ -3605,23 +3561,31 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="17" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C71" s="18"/>
+        <v>134</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
+      <c r="E71" s="19" t="s">
+        <v>135</v>
+      </c>
       <c r="F71" s="19"/>
       <c r="G71" s="19"/>
       <c r="H71" s="18"/>
       <c r="I71" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="J71" s="18"/>
+        <v>136</v>
+      </c>
+      <c r="J71" s="18" t="s">
+        <v>137</v>
+      </c>
       <c r="K71" s="19"/>
-      <c r="L71" s="19"/>
+      <c r="L71" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="M71" s="19"/>
       <c r="N71" s="19"/>
       <c r="O71" s="1"/>
@@ -3629,20 +3593,28 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="17" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C72" s="18"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
+        <v>139</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>140</v>
+      </c>
       <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="19" t="s">
-        <v>148</v>
-      </c>
+      <c r="G72" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I72" s="19"/>
       <c r="J72" s="18"/>
       <c r="K72" s="19"/>
       <c r="L72" s="19"/>
@@ -3653,19 +3625,21 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C73" s="18"/>
+        <v>30</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
       <c r="F73" s="19"/>
       <c r="G73" s="19"/>
       <c r="H73" s="18"/>
       <c r="I73" s="19" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="J73" s="18"/>
       <c r="K73" s="19"/>
@@ -3677,17 +3651,23 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="17" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C74" s="18"/>
+        <v>143</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>144</v>
+      </c>
       <c r="D74" s="19"/>
       <c r="E74" s="19"/>
       <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="18"/>
+      <c r="G74" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H74" s="18" t="s">
+        <v>141</v>
+      </c>
       <c r="I74" s="19"/>
       <c r="J74" s="18"/>
       <c r="K74" s="19"/>
@@ -3696,47 +3676,87 @@
       <c r="N74" s="19"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
+      <c r="AC74" s="1"/>
+      <c r="AD74" s="1"/>
+      <c r="AE74" s="1"/>
+      <c r="AF74" s="1"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="17" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C75" s="18"/>
+        <v>38</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="D75" s="19"/>
       <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
+      <c r="F75" s="19" t="s">
+        <v>146</v>
+      </c>
       <c r="G75" s="19"/>
       <c r="H75" s="18"/>
       <c r="I75" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="J75" s="18"/>
+        <v>147</v>
+      </c>
+      <c r="J75" s="18" t="s">
+        <v>137</v>
+      </c>
       <c r="K75" s="19"/>
-      <c r="L75" s="19"/>
+      <c r="L75" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="M75" s="19"/>
-      <c r="N75" s="19" t="s">
-        <v>152</v>
-      </c>
+      <c r="N75" s="19"/>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+      <c r="AC75" s="1"/>
+      <c r="AD75" s="1"/>
+      <c r="AE75" s="1"/>
+      <c r="AF75" s="1"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="18"/>
+        <v>148</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>149</v>
+      </c>
       <c r="D76" s="19"/>
       <c r="E76" s="19"/>
       <c r="F76" s="19"/>
       <c r="G76" s="19"/>
       <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
+      <c r="I76" s="19"/>
       <c r="J76" s="18"/>
       <c r="K76" s="19"/>
       <c r="L76" s="19"/>
@@ -3744,31 +3764,55 @@
       <c r="N76" s="19"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="1"/>
+      <c r="AB76" s="1"/>
+      <c r="AC76" s="1"/>
+      <c r="AD76" s="1"/>
+      <c r="AE76" s="1"/>
+      <c r="AF76" s="1"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="10"/>
-      <c r="I77" s="10"/>
-      <c r="J77" s="10"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
+      <c r="A77" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G77" s="19"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="19"/>
+      <c r="L77" s="19"/>
+      <c r="M77" s="19"/>
+      <c r="N77" s="19"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="19"/>
@@ -3776,23 +3820,23 @@
       <c r="F78" s="19"/>
       <c r="G78" s="19"/>
       <c r="H78" s="18"/>
-      <c r="I78" s="18" t="s">
-        <v>46</v>
+      <c r="I78" s="19" t="s">
+        <v>151</v>
       </c>
       <c r="J78" s="18"/>
       <c r="K78" s="19"/>
       <c r="L78" s="19"/>
       <c r="M78" s="19"/>
-      <c r="N78" s="18"/>
+      <c r="N78" s="19"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>154</v>
+        <v>60</v>
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="19"/>
@@ -3800,19 +3844,412 @@
       <c r="F79" s="19"/>
       <c r="G79" s="19"/>
       <c r="H79" s="18"/>
-      <c r="I79" s="18" t="s">
-        <v>155</v>
+      <c r="I79" s="19" t="s">
+        <v>152</v>
       </c>
       <c r="J79" s="18"/>
       <c r="K79" s="19"/>
       <c r="L79" s="19"/>
       <c r="M79" s="19"/>
-      <c r="N79" s="18" t="s">
-        <v>155</v>
-      </c>
+      <c r="N79" s="19"/>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
     </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" s="18"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="J80" s="18"/>
+      <c r="K80" s="19"/>
+      <c r="L80" s="19"/>
+      <c r="M80" s="19"/>
+      <c r="N80" s="19"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+    </row>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="A81" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="18"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="19"/>
+      <c r="L81" s="19"/>
+      <c r="M81" s="19"/>
+      <c r="N81" s="19"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="18"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="J82" s="18"/>
+      <c r="K82" s="19"/>
+      <c r="L82" s="19"/>
+      <c r="M82" s="19"/>
+      <c r="N82" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C83" s="18"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="19"/>
+      <c r="L83" s="19"/>
+      <c r="M83" s="19"/>
+      <c r="N83" s="19"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+    </row>
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="A84" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B84" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="18"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="J84" s="18"/>
+      <c r="K84" s="19"/>
+      <c r="L84" s="19"/>
+      <c r="M84" s="19"/>
+      <c r="N84" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+    </row>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B85" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="18"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="J85" s="18"/>
+      <c r="K85" s="19"/>
+      <c r="L85" s="19"/>
+      <c r="M85" s="19"/>
+      <c r="N85" s="18"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+    </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C86" s="18"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="J86" s="18"/>
+      <c r="K86" s="19"/>
+      <c r="L86" s="19"/>
+      <c r="M86" s="19"/>
+      <c r="N86" s="18"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+    </row>
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="A87" s="10"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="10"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+    </row>
+    <row r="88" ht="15.75" customHeight="1">
+      <c r="A88" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G88" s="19"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+      <c r="J88" s="18"/>
+      <c r="K88" s="19"/>
+      <c r="L88" s="19"/>
+      <c r="M88" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="N88" s="19"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+    </row>
+    <row r="89" ht="15.75" customHeight="1">
+      <c r="A89" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G89" s="19"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="19"/>
+      <c r="L89" s="19"/>
+      <c r="M89" s="19"/>
+      <c r="N89" s="19"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+    </row>
+    <row r="90" ht="15.75" customHeight="1">
+      <c r="A90" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="19"/>
+      <c r="L90" s="19"/>
+      <c r="M90" s="19"/>
+      <c r="N90" s="19"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+    </row>
+    <row r="91" ht="15.75" customHeight="1">
+      <c r="A91" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C91" s="18"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="19"/>
+      <c r="L91" s="19"/>
+      <c r="M91" s="19"/>
+      <c r="N91" s="19"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+    </row>
+    <row r="92" ht="15.75" customHeight="1">
+      <c r="A92" s="10"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+    </row>
+    <row r="93" ht="15.75" customHeight="1">
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+    </row>
+    <row r="94" ht="15.75" customHeight="1">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+    </row>
+    <row r="95" ht="15.75" customHeight="1">
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+    </row>
+    <row r="96" ht="15.75" customHeight="1">
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="J96" s="10"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+    </row>
+    <row r="97" ht="15.75" customHeight="1">
+      <c r="A97" s="10"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+    </row>
+    <row r="98" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3822,79 +4259,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="21" disablePrompts="0">
-        <x14:dataValidation xr:uid="{002E004D-00AB-4B20-891F-004A004500D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0092009C-005C-4694-9F2C-00F6002300AC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D2:D8 D10 D21:D22 D24 D31 D37:D46 D74:D75 D76:D77</xm:sqref>
+          <xm:sqref>D2:D8 D10 D24:D25 D35 D41:D53 D81:D82 D83 D87</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A30028-00D9-448B-954E-00E1004600EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{000E009D-0009-41C4-B9A8-0088004700ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A1:A2 A6:A8 A10 A21:A22 A24 A31 A37:A46 A74:A75 A76:A77</xm:sqref>
+          <xm:sqref>A1:A2 A6:A8 A10 A24:A25 A35 A41:A53 A81:A82 A83 A87</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DA00AF-00BC-4A65-99A1-008E003D00CF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00BE007E-0010-467F-82DF-0019009700B5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D47</xm:sqref>
+          <xm:sqref>D54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A9009C-00D1-4CD7-8ABB-007500D30075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{008F00FA-00D9-41E3-9764-00EA004D00BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D50</xm:sqref>
+          <xm:sqref>D57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00810065-00C2-4C91-9E5A-007500E60017}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00390024-00E4-4D4C-9D29-004800F000FD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D52</xm:sqref>
+          <xm:sqref>D59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EE0036-009A-4C1F-A04D-007200460008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{006B00FE-00EE-43B6-A20D-005100AC002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D62</xm:sqref>
+          <xm:sqref>D69</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F70017-007D-4C81-B9D5-00CE00C500D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00E700C3-000E-4328-9495-009000180085}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G63</xm:sqref>
+          <xm:sqref>G70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007500D1-00FA-4B5E-A73B-005E008D0051}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{008300CE-0080-4886-8A07-008600AD005B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G66</xm:sqref>
+          <xm:sqref>G73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001000F2-0012-4608-9EAF-00AD004600E0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{002600F5-0039-4DFA-B8EF-001500160070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -3903,7 +4340,7 @@
           </x14:formula2>
           <xm:sqref>A4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D70067-00DA-48FF-9F7E-00A300650059}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00BA0006-0014-4034-9F12-0016004600E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -3912,25 +4349,25 @@
           </x14:formula2>
           <xm:sqref>A3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00030017-002C-4FB2-A971-00150035009F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0000003B-0081-4AA5-A0ED-00BE0096002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D11:D12 D13:D20 D9</xm:sqref>
+          <xm:sqref>D11:D12 D13:D23 D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004F008D-00FD-406F-88C3-002B007500B9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00B10038-000E-4041-8AC5-003F00C1002E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A11:A12 A13:A20 A9</xm:sqref>
+          <xm:sqref>A11:A12 A13:A23 A9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A6005C-00B3-4D4D-9324-00C1003A0043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{006C0045-0063-4886-A5E8-006D004D0024}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -3939,77 +4376,77 @@
           </x14:formula2>
           <xm:sqref>A5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007900EF-0085-49DA-8A5E-001E00000018}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{009C0098-000E-456F-9988-0007005B00A9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D79</xm:sqref>
+          <xm:sqref>D84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EA0070-00B1-4231-969E-0099000400BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0006004A-002C-45D8-84A6-00F0005600A4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A79</xm:sqref>
+          <xm:sqref>A84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DC00E5-0090-4399-AD73-0002009C0026}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00BC00E0-00F4-4397-BF6E-00BB008900ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D32</xm:sqref>
+          <xm:sqref>D36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007200BD-0085-415A-AE8F-002800A600CA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{005A0034-0020-45B1-B3A6-00DB004E0041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A32</xm:sqref>
+          <xm:sqref>A36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001C00D8-007A-4961-9CD2-008A00DC0085}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00EE0086-00D0-4149-98B8-0038003B007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D78</xm:sqref>
+          <xm:sqref>D26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0049009A-00F9-4622-8E71-00890071007E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00900005-0081-4FA3-8A8C-003700770027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A78</xm:sqref>
+          <xm:sqref>A26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F7000B-00C4-4D2C-96C1-00DF009C0095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00F6005E-00A0-4DB5-993C-00BF00C1000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D23</xm:sqref>
+          <xm:sqref>D88</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003D0037-00CC-49B8-AE5D-000E0033006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D400F9-00F2-4559-84E2-00BE003900EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A23</xm:sqref>
+          <xm:sqref>A88</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4039,7 +4476,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
@@ -4065,13 +4502,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -4113,13 +4550,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -4140,13 +4577,13 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -4166,13 +4603,13 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -4192,13 +4629,13 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -4218,13 +4655,13 @@
     </row>
     <row r="8" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -4244,13 +4681,13 @@
     </row>
     <row r="9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -4290,13 +4727,13 @@
     </row>
     <row r="11" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -4316,13 +4753,13 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -6178,25 +6615,25 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -6220,23 +6657,23 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="24" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-09-01 14-09</v>
+        <v xml:space="preserve">2022-09-28 21-40</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -6267,7 +6704,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1</v>
@@ -6276,22 +6713,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
@@ -6310,13 +6747,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
@@ -6341,13 +6778,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
@@ -6397,13 +6834,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
@@ -6428,13 +6865,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
@@ -6459,13 +6896,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
@@ -6490,13 +6927,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -6521,13 +6958,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -6577,13 +7014,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="34" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -6608,13 +7045,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="34" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -6639,13 +7076,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="34" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -6670,13 +7107,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="34" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -6701,13 +7138,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
@@ -6732,13 +7169,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
@@ -6788,13 +7225,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
@@ -6819,13 +7256,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>225</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>216</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
@@ -6850,13 +7287,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
@@ -6881,13 +7318,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="34" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
@@ -6912,13 +7349,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
@@ -6943,13 +7380,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
@@ -6999,13 +7436,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="34" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
@@ -7030,13 +7467,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="34" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
@@ -7061,13 +7498,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="34" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
@@ -7092,13 +7529,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
@@ -7123,13 +7560,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
@@ -7179,13 +7616,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="34" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
@@ -7210,13 +7647,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="34" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
@@ -7266,121 +7703,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B47" si="0">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B43" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -7391,26 +7828,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -7421,13 +7858,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="35" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="D48" s="35"/>
       <c r="E48" s="35"/>
@@ -7452,13 +7889,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="35" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="C49" s="35" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="D49" s="35"/>
       <c r="E49" s="35"/>
@@ -7484,226 +7921,226 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B51" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C51" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B52" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="C52" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B53" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="C53" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B54" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C54" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B55" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="C55" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="35" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="C58" s="35" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="35" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="35" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="35" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="33" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="33" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="C64" s="35" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="33" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="33" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B66" s="33" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C66" s="35" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="33" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B67" s="33" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B69" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="C69" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B70" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C70" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="B72" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C72" s="36" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="B73" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="C73" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="B74" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C74" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Fix replace_user form so that it does not try to write extra docs
</commit_message>
<xml_diff>
--- a/config/default/forms/app/replace_user.xlsx
+++ b/config/default/forms/app/replace_user.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
   <si>
     <t>type</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t xml:space="preserve">field-list summary</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>note</t>
@@ -282,10 +279,22 @@
     <t>true()</t>
   </si>
   <si>
+    <t xml:space="preserve">. = '1234'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid code. Contact your administrator if you need access to this form.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The code is '1234'</t>
+  </si>
+  <si>
     <t>new_contact</t>
   </si>
   <si>
     <t xml:space="preserve">New User</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>${parent_1_id}</t>
@@ -1294,7 +1303,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{7371A0CD-B85C-02A2-F92F-C7F4F045717A}"/>
+  <person displayName=" " id="{0B2AC635-433A-6A0F-353D-B94AE4049DA1}"/>
 </personList>
 </file>
 
@@ -1710,7 +1719,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="M1" personId="{7371A0CD-B85C-02A2-F92F-C7F4F045717A}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
+  <threadedComment ref="M1" personId="{0B2AC635-433A-6A0F-353D-B94AE4049DA1}" id="{00E10077-0033-4550-BE14-0060002F003A}" done="0">
     <text xml:space="preserve">Comment:
 +marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
@@ -2684,27 +2693,25 @@
       <c r="J36" s="18"/>
       <c r="K36" s="19"/>
       <c r="L36" s="19"/>
-      <c r="M36" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="M36" s="19"/>
       <c r="N36" s="19"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="C37" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>69</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G37" s="19"/>
       <c r="H37" s="18"/>
@@ -2719,13 +2726,13 @@
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="18" t="s">
         <v>71</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>72</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
@@ -2746,20 +2753,26 @@
         <v>34</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="D39" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="18"/>
+      <c r="G39" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>76</v>
+      </c>
       <c r="I39" s="19"/>
-      <c r="J39" s="18"/>
+      <c r="J39" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="K39" s="19"/>
       <c r="L39" s="19"/>
       <c r="M39" s="19"/>
@@ -2812,10 +2825,10 @@
         <v>14</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
@@ -2829,7 +2842,7 @@
       <c r="K42" s="19"/>
       <c r="L42" s="19"/>
       <c r="M42" s="19" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="N42" s="19"/>
       <c r="O42" s="1"/>
@@ -2877,7 +2890,7 @@
       <c r="G44" s="19"/>
       <c r="H44" s="18"/>
       <c r="I44" s="19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J44" s="18"/>
       <c r="K44" s="19"/>
@@ -2899,7 +2912,7 @@
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="18" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F45" s="19" t="s">
         <v>19</v>
@@ -2931,7 +2944,7 @@
       <c r="G46" s="19"/>
       <c r="H46" s="18"/>
       <c r="I46" s="19" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J46" s="18"/>
       <c r="K46" s="19"/>
@@ -2953,7 +2966,7 @@
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
@@ -2983,7 +2996,7 @@
       <c r="G48" s="19"/>
       <c r="H48" s="18"/>
       <c r="I48" s="19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J48" s="18"/>
       <c r="K48" s="19"/>
@@ -3067,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
@@ -3075,7 +3088,7 @@
       <c r="G52" s="19"/>
       <c r="H52" s="18"/>
       <c r="I52" s="20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J52" s="18"/>
       <c r="K52" s="19"/>
@@ -3093,10 +3106,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
@@ -3116,23 +3129,23 @@
         <v>34</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="19"/>
       <c r="F54" s="19"/>
       <c r="G54" s="19" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I54" s="19"/>
       <c r="J54" s="18" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="K54" s="19"/>
       <c r="L54" s="19"/>
@@ -3146,18 +3159,18 @@
         <v>44</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E55" s="19"/>
       <c r="F55" s="19"/>
       <c r="G55" s="19"/>
       <c r="H55" s="18"/>
       <c r="I55" s="19" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J55" s="18"/>
       <c r="K55" s="19"/>
@@ -3172,7 +3185,7 @@
         <v>44</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="19"/>
@@ -3181,7 +3194,7 @@
       <c r="G56" s="19"/>
       <c r="H56" s="18"/>
       <c r="I56" s="19" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J56" s="18"/>
       <c r="K56" s="19"/>
@@ -3196,7 +3209,7 @@
         <v>14</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>16</v>
@@ -3217,30 +3230,30 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="17" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F58" s="19"/>
       <c r="G58" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I58" s="19"/>
       <c r="J58" s="18" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
@@ -3251,17 +3264,17 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D59" s="19"/>
       <c r="E59" s="19" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
@@ -3277,26 +3290,26 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="17" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C60" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="D60" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>105</v>
       </c>
       <c r="F60" s="19"/>
       <c r="G60" s="19" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I60" s="19"/>
       <c r="J60" s="18"/>
@@ -3309,24 +3322,24 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="17" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="19" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F61" s="19"/>
       <c r="G61" s="19" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I61" s="19"/>
       <c r="J61" s="18"/>
@@ -3339,10 +3352,10 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C62" s="18" t="s">
         <v>16</v>
@@ -3350,7 +3363,7 @@
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
       <c r="F62" s="19" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G62" s="19"/>
       <c r="H62" s="18"/>
@@ -3368,7 +3381,7 @@
         <v>44</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="19"/>
@@ -3377,7 +3390,7 @@
       <c r="G63" s="19"/>
       <c r="H63" s="18"/>
       <c r="I63" s="19" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="J63" s="18"/>
       <c r="K63" s="19"/>
@@ -3392,7 +3405,7 @@
         <v>44</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C64" s="18"/>
       <c r="D64" s="19"/>
@@ -3401,7 +3414,7 @@
       <c r="G64" s="19"/>
       <c r="H64" s="18"/>
       <c r="I64" s="19" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="J64" s="18"/>
       <c r="K64" s="19"/>
@@ -3416,7 +3429,7 @@
         <v>44</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="19"/>
@@ -3425,7 +3438,7 @@
       <c r="G65" s="19"/>
       <c r="H65" s="18"/>
       <c r="I65" s="19" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="J65" s="18"/>
       <c r="K65" s="19"/>
@@ -3440,7 +3453,7 @@
         <v>44</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="19"/>
@@ -3449,7 +3462,7 @@
       <c r="G66" s="19"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="J66" s="18"/>
       <c r="K66" s="19"/>
@@ -3464,7 +3477,7 @@
         <v>44</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="19"/>
@@ -3473,7 +3486,7 @@
       <c r="G67" s="19"/>
       <c r="H67" s="18"/>
       <c r="I67" s="19" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J67" s="18"/>
       <c r="K67" s="19"/>
@@ -3485,13 +3498,13 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D68" s="19"/>
       <c r="E68" s="19" t="s">
@@ -3514,7 +3527,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C69" s="18"/>
       <c r="D69" s="19"/>
@@ -3533,20 +3546,20 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D70" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E70" s="19"/>
       <c r="F70" s="19" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G70" s="19"/>
       <c r="H70" s="18"/>
@@ -3561,30 +3574,30 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="17" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C71" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D71" s="19"/>
       <c r="E71" s="19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F71" s="19"/>
       <c r="G71" s="19"/>
       <c r="H71" s="18"/>
       <c r="I71" s="19" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J71" s="18" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="K71" s="19"/>
       <c r="L71" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M71" s="19"/>
       <c r="N71" s="19"/>
@@ -3593,26 +3606,26 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="17" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F72" s="19"/>
       <c r="G72" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="I72" s="19"/>
       <c r="J72" s="18"/>
@@ -3639,7 +3652,7 @@
       <c r="G73" s="19"/>
       <c r="H73" s="18"/>
       <c r="I73" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J73" s="18"/>
       <c r="K73" s="19"/>
@@ -3651,22 +3664,22 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="17" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D74" s="19"/>
       <c r="E74" s="19"/>
       <c r="F74" s="19"/>
       <c r="G74" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H74" s="18" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="I74" s="19"/>
       <c r="J74" s="18"/>
@@ -3695,7 +3708,7 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="17" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B75" s="17" t="s">
         <v>38</v>
@@ -3706,19 +3719,19 @@
       <c r="D75" s="19"/>
       <c r="E75" s="19"/>
       <c r="F75" s="19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G75" s="19"/>
       <c r="H75" s="18"/>
       <c r="I75" s="19" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J75" s="18" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="K75" s="19"/>
       <c r="L75" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M75" s="19"/>
       <c r="N75" s="19"/>
@@ -3746,10 +3759,10 @@
         <v>34</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D76" s="19"/>
       <c r="E76" s="19"/>
@@ -3786,7 +3799,7 @@
         <v>14</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C77" s="18" t="s">
         <v>16</v>
@@ -3821,7 +3834,7 @@
       <c r="G78" s="19"/>
       <c r="H78" s="18"/>
       <c r="I78" s="19" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J78" s="18"/>
       <c r="K78" s="19"/>
@@ -3845,7 +3858,7 @@
       <c r="G79" s="19"/>
       <c r="H79" s="18"/>
       <c r="I79" s="19" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="J79" s="18"/>
       <c r="K79" s="19"/>
@@ -3869,7 +3882,7 @@
       <c r="G80" s="19"/>
       <c r="H80" s="18"/>
       <c r="I80" s="19" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J80" s="18"/>
       <c r="K80" s="19"/>
@@ -3884,7 +3897,7 @@
         <v>32</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C81" s="18"/>
       <c r="D81" s="19"/>
@@ -3906,7 +3919,7 @@
         <v>44</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C82" s="18"/>
       <c r="D82" s="19"/>
@@ -3915,14 +3928,14 @@
       <c r="G82" s="19"/>
       <c r="H82" s="18"/>
       <c r="I82" s="19" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="J82" s="18"/>
       <c r="K82" s="19"/>
       <c r="L82" s="19"/>
       <c r="M82" s="19"/>
       <c r="N82" s="19" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
@@ -3932,7 +3945,7 @@
         <v>32</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C83" s="18"/>
       <c r="D83" s="19"/>
@@ -3954,7 +3967,7 @@
         <v>44</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C84" s="18"/>
       <c r="D84" s="19"/>
@@ -3963,14 +3976,14 @@
       <c r="G84" s="19"/>
       <c r="H84" s="18"/>
       <c r="I84" s="18" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J84" s="18"/>
       <c r="K84" s="19"/>
       <c r="L84" s="19"/>
       <c r="M84" s="19"/>
       <c r="N84" s="18" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
@@ -3980,7 +3993,7 @@
         <v>44</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C85" s="18"/>
       <c r="D85" s="19"/>
@@ -3989,7 +4002,7 @@
       <c r="G85" s="19"/>
       <c r="H85" s="18"/>
       <c r="I85" s="18" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="J85" s="18"/>
       <c r="K85" s="19"/>
@@ -4004,7 +4017,7 @@
         <v>44</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C86" s="18"/>
       <c r="D86" s="19"/>
@@ -4013,7 +4026,7 @@
       <c r="G86" s="19"/>
       <c r="H86" s="18"/>
       <c r="I86" s="18" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J86" s="18"/>
       <c r="K86" s="19"/>
@@ -4046,7 +4059,7 @@
         <v>14</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C88" s="18" t="s">
         <v>16</v>
@@ -4062,27 +4075,25 @@
       <c r="J88" s="18"/>
       <c r="K88" s="19"/>
       <c r="L88" s="19"/>
-      <c r="M88" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="M88" s="19"/>
       <c r="N88" s="19"/>
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B89" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="C89" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="C89" s="18" t="s">
-        <v>69</v>
       </c>
       <c r="D89" s="19"/>
       <c r="E89" s="19"/>
       <c r="F89" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G89" s="19"/>
       <c r="H89" s="18"/>
@@ -4097,13 +4108,13 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D90" s="19"/>
       <c r="E90" s="19"/>
@@ -4124,7 +4135,7 @@
         <v>32</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C91" s="18"/>
       <c r="D91" s="19"/>
@@ -4259,7 +4270,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="21" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0092009C-005C-4694-9F2C-00F6002300AC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D000D8-00EC-4519-8A0B-00ED009E00EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4268,7 +4279,7 @@
           </x14:formula2>
           <xm:sqref>D2:D8 D10 D24:D25 D35 D41:D53 D81:D82 D83 D87</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000E009D-0009-41C4-B9A8-0088004700ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00310038-00DE-4D8D-B88E-00550045006D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4277,7 +4288,7 @@
           </x14:formula2>
           <xm:sqref>A1:A2 A6:A8 A10 A24:A25 A35 A41:A53 A81:A82 A83 A87</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00BE007E-0010-467F-82DF-0019009700B5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{002100FC-0098-42EF-8BE3-00BB00900082}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4286,7 +4297,7 @@
           </x14:formula2>
           <xm:sqref>D54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008F00FA-00D9-41E3-9764-00EA004D00BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{005300E7-0007-4564-989B-00140049002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4295,7 +4306,7 @@
           </x14:formula2>
           <xm:sqref>D57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00390024-00E4-4D4C-9D29-004800F000FD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{002D008E-0035-49C0-87CA-005D00D400A5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4304,7 +4315,7 @@
           </x14:formula2>
           <xm:sqref>D59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006B00FE-00EE-43B6-A20D-005100AC002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00440039-0002-47C1-9242-00CA00E3007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4313,7 +4324,7 @@
           </x14:formula2>
           <xm:sqref>D69</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E700C3-000E-4328-9495-009000180085}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00B700A3-00A6-418C-AFDC-00A900F40092}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4322,7 +4333,7 @@
           </x14:formula2>
           <xm:sqref>G70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008300CE-0080-4886-8A07-008600AD005B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{006400A7-0032-48BF-932B-004B00B700EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4331,7 +4342,7 @@
           </x14:formula2>
           <xm:sqref>G73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002600F5-0039-4DFA-B8EF-001500160070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00B500F5-00B1-413A-B87D-002300040007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4340,7 +4351,7 @@
           </x14:formula2>
           <xm:sqref>A4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00BA0006-0014-4034-9F12-0016004600E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{0054009A-00F6-4BC2-B6F1-00BD00BF0095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4349,7 +4360,7 @@
           </x14:formula2>
           <xm:sqref>A3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0000003B-0081-4AA5-A0ED-00BE0096002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D9002E-0079-46EA-B3A2-00D6004400EA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4358,7 +4369,7 @@
           </x14:formula2>
           <xm:sqref>D11:D12 D13:D23 D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B10038-000E-4041-8AC5-003F00C1002E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00B20054-00D4-47AB-8393-002D00790030}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4367,7 +4378,7 @@
           </x14:formula2>
           <xm:sqref>A11:A12 A13:A23 A9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006C0045-0063-4886-A5E8-006D004D0024}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00BD00C8-006F-4128-A4C6-007A007700D9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4376,7 +4387,7 @@
           </x14:formula2>
           <xm:sqref>A5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009C0098-000E-456F-9988-0007005B00A9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00650045-00AE-4E7B-B13B-00140085002E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4385,7 +4396,7 @@
           </x14:formula2>
           <xm:sqref>D84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0006004A-002C-45D8-84A6-00F0005600A4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00C400B6-000A-4494-B798-00DC001B00F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4394,7 +4405,7 @@
           </x14:formula2>
           <xm:sqref>A84</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00BC00E0-00F4-4397-BF6E-00BB008900ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{009100E1-0008-46B8-956E-00B400E30083}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4403,7 +4414,7 @@
           </x14:formula2>
           <xm:sqref>D36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005A0034-0020-45B1-B3A6-00DB004E0041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00F90065-006C-4DCA-87E1-00A4005B007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4412,7 +4423,7 @@
           </x14:formula2>
           <xm:sqref>A36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EE0086-00D0-4149-98B8-0038003B007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{001A00D1-002E-4927-ADAA-00E9007900F1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4421,7 +4432,7 @@
           </x14:formula2>
           <xm:sqref>D26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00900005-0081-4FA3-8A8C-003700770027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{003C00A2-00AC-4EB8-AFC7-00F600AE0049}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4430,7 +4441,7 @@
           </x14:formula2>
           <xm:sqref>A26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F6005E-00A0-4DB5-993C-00BF00C1000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00DD00D9-004C-4A5E-9C03-006B00560090}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -4439,7 +4450,7 @@
           </x14:formula2>
           <xm:sqref>D88</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D400F9-00F2-4559-84E2-00BE003900EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00DA006B-00E9-48E9-9A4D-0084007D00A8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -4476,7 +4487,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
@@ -4502,13 +4513,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -4550,13 +4561,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -4577,13 +4588,13 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -4603,13 +4614,13 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -4629,13 +4640,13 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -4655,13 +4666,13 @@
     </row>
     <row r="8" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -4681,13 +4692,13 @@
     </row>
     <row r="9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -4727,13 +4738,13 @@
     </row>
     <row r="11" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -4753,13 +4764,13 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -6615,25 +6626,25 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -6657,23 +6668,23 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="24" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-09-28 21-40</v>
+        <v xml:space="preserve">2022-11-23 12-06</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -6704,7 +6715,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1</v>
@@ -6713,22 +6724,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
@@ -6747,13 +6758,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
@@ -6778,13 +6789,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
@@ -6834,13 +6845,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
@@ -6865,13 +6876,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
@@ -6896,13 +6907,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
@@ -6927,13 +6938,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -6958,13 +6969,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -7014,13 +7025,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="34" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -7045,13 +7056,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="34" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -7076,13 +7087,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="34" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -7107,13 +7118,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="34" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -7138,13 +7149,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
@@ -7169,13 +7180,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
@@ -7225,13 +7236,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
@@ -7256,13 +7267,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="34" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
@@ -7287,13 +7298,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
@@ -7318,13 +7329,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="34" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
@@ -7349,13 +7360,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
@@ -7380,13 +7391,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
@@ -7436,13 +7447,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="34" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
@@ -7467,13 +7478,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="34" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
@@ -7498,13 +7509,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="34" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
@@ -7529,13 +7540,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
@@ -7560,13 +7571,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
@@ -7616,13 +7627,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="34" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
@@ -7647,13 +7658,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="34" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
@@ -7703,121 +7714,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B47" si="0">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C43" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -7828,26 +7839,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -7858,13 +7869,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="35" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D48" s="35"/>
       <c r="E48" s="35"/>
@@ -7889,13 +7900,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="35" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C49" s="35" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D49" s="35"/>
       <c r="E49" s="35"/>
@@ -7921,226 +7932,226 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B51" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C51" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B52" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C52" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B53" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C53" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B54" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C54" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B55" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C55" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B56" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C56" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="35" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C58" s="35" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="35" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="35" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="35" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="33" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="33" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C64" s="35" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="33" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="33" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B66" s="33" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C66" s="35" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="33" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B67" s="33" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B69" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C69" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B70" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C70" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B72" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C72" s="36" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B73" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C73" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B74" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C74" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>